<commit_message>
Fix Laporan Belanja Persediaan
</commit_message>
<xml_diff>
--- a/utility/optbs/template/belanja_persediaan_2.xlsx
+++ b/utility/optbs/template/belanja_persediaan_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>SKPD</t>
   </si>
@@ -52,6 +52,9 @@
     <t>NO</t>
   </si>
   <si>
+    <t>NOMOR DOKUMEN</t>
+  </si>
+  <si>
     <t>REK. BELANJA</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>[a.no;ope=tbs:num;block=row;] </t>
   </si>
   <si>
+    <t>[a.no_dok]</t>
+  </si>
+  <si>
     <t>[a.kode_rekening]</t>
   </si>
   <si>
@@ -86,6 +92,12 @@
   </si>
   <si>
     <t>[a.nm_perk]</t>
+  </si>
+  <si>
+    <t>[c.total_persediaan; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[c.total_non_persediaan; ope=tbs:num]</t>
   </si>
   <si>
     <t>Kota Pekalongan, [b.tanggal_cetak]</t>
@@ -244,7 +256,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,10 +299,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -430,24 +438,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:65536"/>
+  <dimension ref="1:24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1018" min="9" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1020" min="1019" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1022" min="1021" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1021" min="1020" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1023" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,14 +463,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="0"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
       <c r="K1" s="0"/>
@@ -1473,20 +1481,21 @@
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="0"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
@@ -2497,20 +2506,21 @@
       <c r="AMB2" s="0"/>
       <c r="AMC2" s="0"/>
       <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="0"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
@@ -3521,17 +3531,18 @@
       <c r="AMB3" s="0"/>
       <c r="AMC3" s="0"/>
       <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="0"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
@@ -4541,6 +4552,7 @@
       <c r="AMB4" s="0"/>
       <c r="AMC4" s="0"/>
       <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -4553,7 +4565,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="0"/>
+      <c r="I5" s="6"/>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
       <c r="L5" s="0"/>
@@ -5563,6 +5575,7 @@
       <c r="AMB5" s="0"/>
       <c r="AMC5" s="0"/>
       <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -5575,7 +5588,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="0"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
       <c r="L6" s="0"/>
@@ -6585,6 +6598,7 @@
       <c r="AMB6" s="0"/>
       <c r="AMC6" s="0"/>
       <c r="AMD6" s="0"/>
+      <c r="AME6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
@@ -6597,7 +6611,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="0"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
@@ -7607,6 +7621,7 @@
       <c r="AMB7" s="0"/>
       <c r="AMC7" s="0"/>
       <c r="AMD7" s="0"/>
+      <c r="AME7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
@@ -8627,6 +8642,7 @@
       <c r="AMB8" s="0"/>
       <c r="AMC8" s="0"/>
       <c r="AMD8" s="0"/>
+      <c r="AME8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
@@ -9647,6 +9663,7 @@
       <c r="AMB9" s="0"/>
       <c r="AMC9" s="0"/>
       <c r="AMD9" s="0"/>
+      <c r="AME9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="30.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
@@ -9673,7 +9690,9 @@
       <c r="H10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="0"/>
+      <c r="I10" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
@@ -10683,6 +10702,7 @@
       <c r="AMB10" s="0"/>
       <c r="AMC10" s="0"/>
       <c r="AMD10" s="0"/>
+      <c r="AME10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="n">
@@ -10709,7 +10729,9 @@
       <c r="H11" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="I11" s="0"/>
+      <c r="I11" s="8" t="n">
+        <v>9</v>
+      </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
@@ -11719,36 +11741,39 @@
       <c r="AMB11" s="0"/>
       <c r="AMC11" s="0"/>
       <c r="AMD11" s="0"/>
+      <c r="AME11" s="0"/>
     </row>
-    <row r="12" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="13" customFormat="true" ht="71.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="13" t="e">
+      <c r="E12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="12" t="e">
         <f aca="false">VALUE([a.total_harga])</f>
-        <v>#N/A</v>
+        <v>#NAME?</v>
       </c>
-      <c r="G12" s="13" t="e">
+      <c r="H12" s="12" t="e">
         <f aca="false">VALUE([a.nilai_kontrak])</f>
-        <v>#N/A</v>
+        <v>#NAME?</v>
       </c>
-      <c r="H12" s="13" t="e">
+      <c r="I12" s="12" t="e">
         <f aca="true">INDIRECT( "F" &amp; ROW() )+INDIRECT( "G" &amp; ROW() )</f>
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
-      <c r="AME12" s="0"/>
       <c r="AMF12" s="0"/>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -11756,17 +11781,24 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="7" t="s">
-        <v>16</v>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="7" t="s">
+        <v>17</v>
       </c>
-      <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="0"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="15" t="e">
+        <f aca="true">INDIRECT( "G" &amp; ROW() )+INDIRECT( "H" &amp; ROW() )</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
       <c r="L13" s="0"/>
@@ -12776,15 +12808,16 @@
       <c r="AMB13" s="0"/>
       <c r="AMC13" s="0"/>
       <c r="AMD13" s="0"/>
+      <c r="AME13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="0"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
@@ -13796,22 +13829,23 @@
       <c r="AMB14" s="0"/>
       <c r="AMC14" s="0"/>
       <c r="AMD14" s="0"/>
+      <c r="AME14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="2" t="s">
-        <v>22</v>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="2" t="s">
+        <v>26</v>
       </c>
-      <c r="H15" s="0"/>
       <c r="I15" s="0"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
       <c r="M15" s="0"/>
       <c r="N15" s="0"/>
       <c r="O15" s="0"/>
@@ -14818,10 +14852,11 @@
       <c r="AMB15" s="0"/>
       <c r="AMC15" s="0"/>
       <c r="AMD15" s="0"/>
+      <c r="AME15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -14829,8 +14864,8 @@
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="18"/>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
       <c r="L16" s="0"/>
@@ -15840,22 +15875,23 @@
       <c r="AMB16" s="0"/>
       <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
+      <c r="AME16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="0"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="0"/>
-      <c r="E17" s="19" t="s">
-        <v>25</v>
+      <c r="E17" s="0"/>
+      <c r="F17" s="18" t="s">
+        <v>29</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>26</v>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>30</v>
       </c>
-      <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -16866,18 +16902,19 @@
       <c r="AMB17" s="0"/>
       <c r="AMC17" s="0"/>
       <c r="AMD17" s="0"/>
+      <c r="AME17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="0"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="0"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="0"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="0"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -17888,16 +17925,17 @@
       <c r="AMB18" s="0"/>
       <c r="AMC18" s="0"/>
       <c r="AMD18" s="0"/>
+      <c r="AME18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20"/>
-      <c r="B19" s="0"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="0"/>
       <c r="D19" s="0"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="0"/>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
@@ -18908,16 +18946,17 @@
       <c r="AMB19" s="0"/>
       <c r="AMC19" s="0"/>
       <c r="AMD19" s="0"/>
+      <c r="AME19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
-      <c r="B20" s="0"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="0"/>
       <c r="D20" s="0"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="0"/>
       <c r="J20" s="0"/>
       <c r="K20" s="0"/>
@@ -19928,16 +19967,17 @@
       <c r="AMB20" s="0"/>
       <c r="AMC20" s="0"/>
       <c r="AMD20" s="0"/>
+      <c r="AME20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20"/>
-      <c r="B21" s="0"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="0"/>
       <c r="D21" s="0"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
@@ -20948,16 +20988,17 @@
       <c r="AMB21" s="0"/>
       <c r="AMC21" s="0"/>
       <c r="AMD21" s="0"/>
+      <c r="AME21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20"/>
-      <c r="B22" s="0"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="0"/>
       <c r="D22" s="0"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
@@ -21968,64 +22009,64 @@
       <c r="AMB22" s="0"/>
       <c r="AMC22" s="0"/>
       <c r="AMD22" s="0"/>
+      <c r="AME22" s="0"/>
     </row>
-    <row r="23" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="s">
-        <v>28</v>
+    <row r="23" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="20" t="s">
+        <v>32</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="19" t="s">
-        <v>29</v>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="18" t="s">
+        <v>33</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21" t="s">
-        <v>30</v>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20" t="s">
+        <v>34</v>
       </c>
-      <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
-      <c r="K23" s="23"/>
-      <c r="AME23" s="23"/>
-      <c r="AMF23" s="23"/>
-      <c r="AMG23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="22"/>
+      <c r="AMF23" s="22"/>
+      <c r="AMG23" s="22"/>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="19" t="s">
-        <v>32</v>
+      <c r="B24" s="3"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="18" t="s">
+        <v>36</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3" t="s">
-        <v>33</v>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>37</v>
       </c>
-      <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
-      <c r="K24" s="26"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="25"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:I7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.379861111111111" right="0.379861111111111" top="0.645138888888889" bottom="0.645138888888889" header="0.379861111111111" footer="0.379861111111111"/>

</xml_diff>

<commit_message>
Fix Laporan Belanja Persediaan Per Rekening
</commit_message>
<xml_diff>
--- a/utility/optbs/template/belanja_persediaan_2.xlsx
+++ b/utility/optbs/template/belanja_persediaan_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,139 +13,148 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
-    <t>SKPD</t>
+    <t xml:space="preserve">SKPD</t>
   </si>
   <si>
-    <t>: [b.nama_skpd]</t>
+    <t xml:space="preserve">: [b.nama_skpd]</t>
   </si>
   <si>
-    <t>Provinsi</t>
+    <t xml:space="preserve">Provinsi</t>
   </si>
   <si>
-    <t>: Jawa Tengah</t>
+    <t xml:space="preserve">: Jawa Tengah</t>
   </si>
   <si>
-    <t>Kabupaten / Kota</t>
+    <t xml:space="preserve">Kabupaten / Kota</t>
   </si>
   <si>
-    <t>:Kota Pekalongan</t>
+    <t xml:space="preserve">:Kota Pekalongan</t>
   </si>
   <si>
-    <t>LAPORAN POSISI PERSEDIAAN DI NERACA PER REKENING</t>
+    <t xml:space="preserve">LAPORAN POSISI PERSEDIAAN DI NERACA PER REKENING</t>
   </si>
   <si>
-    <t>UNTUK PERIODE YANG BERAKHIR PADA [a.tanggal]</t>
+    <t xml:space="preserve">UNTUK PERIODE YANG BERAKHIR PADA [a.tanggal]</t>
   </si>
   <si>
-    <t>TAHUN ANGGARAN [a.tahun]</t>
+    <t xml:space="preserve">TAHUN ANGGARAN [a.tahun]</t>
   </si>
   <si>
-    <t>NO</t>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t>REK. BELANJA</t>
+    <t xml:space="preserve">REK. BELANJA</t>
   </si>
   <si>
-    <t>URAIAN REK. BELANJA</t>
+    <t xml:space="preserve">URAIAN REK. BELANJA</t>
   </si>
   <si>
-    <t>REKENING PERSEDIAAN</t>
+    <t xml:space="preserve">REKENING PERSEDIAAN</t>
   </si>
   <si>
-    <t>URAIAN REKENING PERSEDIAAN</t>
+    <t xml:space="preserve">URAIAN REKENING PERSEDIAAN</t>
   </si>
   <si>
-    <t>NILAI PERSEDIAAN</t>
+    <t xml:space="preserve">NILAI PERSEDIAAN</t>
   </si>
   <si>
-    <t>NILAI NON PERSEDIAAN</t>
+    <t xml:space="preserve">NILAI NON PERSEDIAAN</t>
   </si>
   <si>
-    <t>TOTAL</t>
+    <t xml:space="preserve">TOTAL</t>
   </si>
   <si>
-    <t>SUBTOTAL</t>
+    <t xml:space="preserve"> [a.nm_satker; block=row; when [a.cetak_satker]=1]</t>
   </si>
   <si>
-    <t> [a.subTot_persediaan; ope=tbs:num;  block=row; when [a.cetak_subtotal]=1]</t>
+    <t xml:space="preserve">[a.no; block=row;  when [a.cetak_rekening]=1] </t>
   </si>
   <si>
-    <t> [a.subTot_nonPersediaan; ope=tbs:num; ]</t>
+    <t xml:space="preserve">[a.kode_rekening]</t>
   </si>
   <si>
-    <t>[a.no;ope=tbs:num;block=row;] </t>
+    <t xml:space="preserve">[a.nama_rekening]</t>
   </si>
   <si>
-    <t>[a.kode_rekening]</t>
+    <t xml:space="preserve">[a.total_harga; ope=tbs:num;]</t>
   </si>
   <si>
-    <t>[a.nama_rekening]</t>
+    <t xml:space="preserve">[a.nilai_kontrak; ope=tbs:num;]</t>
   </si>
   <si>
-    <t>[a.kd_perk]</t>
+    <t xml:space="preserve">[a.grand_total; ope=tbs:num;]</t>
   </si>
   <si>
-    <t>[a.nm_perk]</t>
+    <t xml:space="preserve">[a.no; block=row;  when [a.cetak_detail]=1] </t>
   </si>
   <si>
-    <t>[a.total_harga; ope=tbs:num;]</t>
+    <t xml:space="preserve">[a.kd_perk]</t>
   </si>
   <si>
-    <t>[a.nilai_kontrak; ope=tbs:num;]</t>
+    <t xml:space="preserve">[a.nm_perk]</t>
   </si>
   <si>
-    <t> [a.subTot_persediaan; ope=tbs:num;  block=row; when [a.cetak_subtotal]=2]</t>
+    <t xml:space="preserve">[a.no]</t>
   </si>
   <si>
-    <t>[c.total_persediaan; ope=tbs:num]</t>
+    <t xml:space="preserve">SUBTOTAL</t>
   </si>
   <si>
-    <t>[c.total_non_persediaan; ope=tbs:num]</t>
+    <t xml:space="preserve"> [a.total_harga; ope=tbs:num;  block=row; when [a.cetak_subtotal]=1]</t>
   </si>
   <si>
-    <t>Kota Pekalongan, [b.tanggal_cetak]</t>
+    <t xml:space="preserve"> [a.nilai_kontrak; ope=tbs:num; ]</t>
   </si>
   <si>
-    <t>Mengetahui</t>
+    <t xml:space="preserve">[c.total_persediaan; ope=tbs:num]</t>
   </si>
   <si>
-    <t>An Pengguna / Kuasa Pengguna Barang</t>
+    <t xml:space="preserve">[c.total_non_persediaan; ope=tbs:num]</t>
   </si>
   <si>
-    <t>Pengurus Barang</t>
+    <t xml:space="preserve">Kota Pekalongan, [b.tanggal_cetak]</t>
   </si>
   <si>
-    <t>Pembantu Pengurus Barang</t>
+    <t xml:space="preserve">Mengetahui</t>
   </si>
   <si>
-    <t>Pejabat Penatausahaan Pengguna Barang</t>
+    <t xml:space="preserve">An Pengguna / Kuasa Pengguna Barang</t>
   </si>
   <si>
-    <t>([b.nama_atasan])</t>
+    <t xml:space="preserve">Pengurus Barang</t>
   </si>
   <si>
-    <t>……………………………………</t>
+    <t xml:space="preserve">Pembantu Pengurus Barang</t>
   </si>
   <si>
-    <t>([b.nama_penyimpan_barang])</t>
+    <t xml:space="preserve">Pejabat Penatausahaan Pengguna Barang</t>
   </si>
   <si>
-    <t>NIP. [b.nip_atasan]</t>
+    <t xml:space="preserve">([b.nama_atasan])</t>
   </si>
   <si>
-    <t>NIP ………………………………</t>
+    <t xml:space="preserve">……………………………………</t>
   </si>
   <si>
-    <t>NIP. [b.nip_penyimpan_barang]</t>
+    <t xml:space="preserve">([b.nama_penyimpan_barang])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIP. [b.nip_atasan]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIP ………………………………</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIP. [b.nip_penyimpan_barang]</t>
   </si>
 </sst>
 </file>
@@ -153,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="10">
@@ -229,12 +238,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -244,27 +253,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
@@ -296,7 +284,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,36 +317,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -370,31 +338,43 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -449,7 +429,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -471,7 +451,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -514,24 +494,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:26"/>
+  <dimension ref="A1:AMJ27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1018" min="9" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1020" min="1019" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1022" min="1021" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="6.0765306122449"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="9" style="1" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1019" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="6.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11804,2114 +11784,86 @@
       <c r="AMC11" s="0"/>
       <c r="AMD11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
+    <row r="12" s="10" customFormat="true" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" s="14" customFormat="true" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="15" t="e">
-        <f aca="true">INDIRECT( "G" &amp; ROW() )+INDIRECT( "F" &amp; ROW() )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I12" s="0"/>
-      <c r="J12" s="0"/>
-      <c r="K12" s="0"/>
-      <c r="L12" s="0"/>
-      <c r="M12" s="0"/>
-      <c r="N12" s="0"/>
-      <c r="O12" s="0"/>
-      <c r="P12" s="0"/>
-      <c r="Q12" s="0"/>
-      <c r="R12" s="0"/>
-      <c r="S12" s="0"/>
-      <c r="T12" s="0"/>
-      <c r="U12" s="0"/>
-      <c r="V12" s="0"/>
-      <c r="W12" s="0"/>
-      <c r="X12" s="0"/>
-      <c r="Y12" s="0"/>
-      <c r="Z12" s="0"/>
-      <c r="AA12" s="0"/>
-      <c r="AB12" s="0"/>
-      <c r="AC12" s="0"/>
-      <c r="AD12" s="0"/>
-      <c r="AE12" s="0"/>
-      <c r="AF12" s="0"/>
-      <c r="AG12" s="0"/>
-      <c r="AH12" s="0"/>
-      <c r="AI12" s="0"/>
-      <c r="AJ12" s="0"/>
-      <c r="AK12" s="0"/>
-      <c r="AL12" s="0"/>
-      <c r="AM12" s="0"/>
-      <c r="AN12" s="0"/>
-      <c r="AO12" s="0"/>
-      <c r="AP12" s="0"/>
-      <c r="AQ12" s="0"/>
-      <c r="AR12" s="0"/>
-      <c r="AS12" s="0"/>
-      <c r="AT12" s="0"/>
-      <c r="AU12" s="0"/>
-      <c r="AV12" s="0"/>
-      <c r="AW12" s="0"/>
-      <c r="AX12" s="0"/>
-      <c r="AY12" s="0"/>
-      <c r="AZ12" s="0"/>
-      <c r="BA12" s="0"/>
-      <c r="BB12" s="0"/>
-      <c r="BC12" s="0"/>
-      <c r="BD12" s="0"/>
-      <c r="BE12" s="0"/>
-      <c r="BF12" s="0"/>
-      <c r="BG12" s="0"/>
-      <c r="BH12" s="0"/>
-      <c r="BI12" s="0"/>
-      <c r="BJ12" s="0"/>
-      <c r="BK12" s="0"/>
-      <c r="BL12" s="0"/>
-      <c r="BM12" s="0"/>
-      <c r="BN12" s="0"/>
-      <c r="BO12" s="0"/>
-      <c r="BP12" s="0"/>
-      <c r="BQ12" s="0"/>
-      <c r="BR12" s="0"/>
-      <c r="BS12" s="0"/>
-      <c r="BT12" s="0"/>
-      <c r="BU12" s="0"/>
-      <c r="BV12" s="0"/>
-      <c r="BW12" s="0"/>
-      <c r="BX12" s="0"/>
-      <c r="BY12" s="0"/>
-      <c r="BZ12" s="0"/>
-      <c r="CA12" s="0"/>
-      <c r="CB12" s="0"/>
-      <c r="CC12" s="0"/>
-      <c r="CD12" s="0"/>
-      <c r="CE12" s="0"/>
-      <c r="CF12" s="0"/>
-      <c r="CG12" s="0"/>
-      <c r="CH12" s="0"/>
-      <c r="CI12" s="0"/>
-      <c r="CJ12" s="0"/>
-      <c r="CK12" s="0"/>
-      <c r="CL12" s="0"/>
-      <c r="CM12" s="0"/>
-      <c r="CN12" s="0"/>
-      <c r="CO12" s="0"/>
-      <c r="CP12" s="0"/>
-      <c r="CQ12" s="0"/>
-      <c r="CR12" s="0"/>
-      <c r="CS12" s="0"/>
-      <c r="CT12" s="0"/>
-      <c r="CU12" s="0"/>
-      <c r="CV12" s="0"/>
-      <c r="CW12" s="0"/>
-      <c r="CX12" s="0"/>
-      <c r="CY12" s="0"/>
-      <c r="CZ12" s="0"/>
-      <c r="DA12" s="0"/>
-      <c r="DB12" s="0"/>
-      <c r="DC12" s="0"/>
-      <c r="DD12" s="0"/>
-      <c r="DE12" s="0"/>
-      <c r="DF12" s="0"/>
-      <c r="DG12" s="0"/>
-      <c r="DH12" s="0"/>
-      <c r="DI12" s="0"/>
-      <c r="DJ12" s="0"/>
-      <c r="DK12" s="0"/>
-      <c r="DL12" s="0"/>
-      <c r="DM12" s="0"/>
-      <c r="DN12" s="0"/>
-      <c r="DO12" s="0"/>
-      <c r="DP12" s="0"/>
-      <c r="DQ12" s="0"/>
-      <c r="DR12" s="0"/>
-      <c r="DS12" s="0"/>
-      <c r="DT12" s="0"/>
-      <c r="DU12" s="0"/>
-      <c r="DV12" s="0"/>
-      <c r="DW12" s="0"/>
-      <c r="DX12" s="0"/>
-      <c r="DY12" s="0"/>
-      <c r="DZ12" s="0"/>
-      <c r="EA12" s="0"/>
-      <c r="EB12" s="0"/>
-      <c r="EC12" s="0"/>
-      <c r="ED12" s="0"/>
-      <c r="EE12" s="0"/>
-      <c r="EF12" s="0"/>
-      <c r="EG12" s="0"/>
-      <c r="EH12" s="0"/>
-      <c r="EI12" s="0"/>
-      <c r="EJ12" s="0"/>
-      <c r="EK12" s="0"/>
-      <c r="EL12" s="0"/>
-      <c r="EM12" s="0"/>
-      <c r="EN12" s="0"/>
-      <c r="EO12" s="0"/>
-      <c r="EP12" s="0"/>
-      <c r="EQ12" s="0"/>
-      <c r="ER12" s="0"/>
-      <c r="ES12" s="0"/>
-      <c r="ET12" s="0"/>
-      <c r="EU12" s="0"/>
-      <c r="EV12" s="0"/>
-      <c r="EW12" s="0"/>
-      <c r="EX12" s="0"/>
-      <c r="EY12" s="0"/>
-      <c r="EZ12" s="0"/>
-      <c r="FA12" s="0"/>
-      <c r="FB12" s="0"/>
-      <c r="FC12" s="0"/>
-      <c r="FD12" s="0"/>
-      <c r="FE12" s="0"/>
-      <c r="FF12" s="0"/>
-      <c r="FG12" s="0"/>
-      <c r="FH12" s="0"/>
-      <c r="FI12" s="0"/>
-      <c r="FJ12" s="0"/>
-      <c r="FK12" s="0"/>
-      <c r="FL12" s="0"/>
-      <c r="FM12" s="0"/>
-      <c r="FN12" s="0"/>
-      <c r="FO12" s="0"/>
-      <c r="FP12" s="0"/>
-      <c r="FQ12" s="0"/>
-      <c r="FR12" s="0"/>
-      <c r="FS12" s="0"/>
-      <c r="FT12" s="0"/>
-      <c r="FU12" s="0"/>
-      <c r="FV12" s="0"/>
-      <c r="FW12" s="0"/>
-      <c r="FX12" s="0"/>
-      <c r="FY12" s="0"/>
-      <c r="FZ12" s="0"/>
-      <c r="GA12" s="0"/>
-      <c r="GB12" s="0"/>
-      <c r="GC12" s="0"/>
-      <c r="GD12" s="0"/>
-      <c r="GE12" s="0"/>
-      <c r="GF12" s="0"/>
-      <c r="GG12" s="0"/>
-      <c r="GH12" s="0"/>
-      <c r="GI12" s="0"/>
-      <c r="GJ12" s="0"/>
-      <c r="GK12" s="0"/>
-      <c r="GL12" s="0"/>
-      <c r="GM12" s="0"/>
-      <c r="GN12" s="0"/>
-      <c r="GO12" s="0"/>
-      <c r="GP12" s="0"/>
-      <c r="GQ12" s="0"/>
-      <c r="GR12" s="0"/>
-      <c r="GS12" s="0"/>
-      <c r="GT12" s="0"/>
-      <c r="GU12" s="0"/>
-      <c r="GV12" s="0"/>
-      <c r="GW12" s="0"/>
-      <c r="GX12" s="0"/>
-      <c r="GY12" s="0"/>
-      <c r="GZ12" s="0"/>
-      <c r="HA12" s="0"/>
-      <c r="HB12" s="0"/>
-      <c r="HC12" s="0"/>
-      <c r="HD12" s="0"/>
-      <c r="HE12" s="0"/>
-      <c r="HF12" s="0"/>
-      <c r="HG12" s="0"/>
-      <c r="HH12" s="0"/>
-      <c r="HI12" s="0"/>
-      <c r="HJ12" s="0"/>
-      <c r="HK12" s="0"/>
-      <c r="HL12" s="0"/>
-      <c r="HM12" s="0"/>
-      <c r="HN12" s="0"/>
-      <c r="HO12" s="0"/>
-      <c r="HP12" s="0"/>
-      <c r="HQ12" s="0"/>
-      <c r="HR12" s="0"/>
-      <c r="HS12" s="0"/>
-      <c r="HT12" s="0"/>
-      <c r="HU12" s="0"/>
-      <c r="HV12" s="0"/>
-      <c r="HW12" s="0"/>
-      <c r="HX12" s="0"/>
-      <c r="HY12" s="0"/>
-      <c r="HZ12" s="0"/>
-      <c r="IA12" s="0"/>
-      <c r="IB12" s="0"/>
-      <c r="IC12" s="0"/>
-      <c r="ID12" s="0"/>
-      <c r="IE12" s="0"/>
-      <c r="IF12" s="0"/>
-      <c r="IG12" s="0"/>
-      <c r="IH12" s="0"/>
-      <c r="II12" s="0"/>
-      <c r="IJ12" s="0"/>
-      <c r="IK12" s="0"/>
-      <c r="IL12" s="0"/>
-      <c r="IM12" s="0"/>
-      <c r="IN12" s="0"/>
-      <c r="IO12" s="0"/>
-      <c r="IP12" s="0"/>
-      <c r="IQ12" s="0"/>
-      <c r="IR12" s="0"/>
-      <c r="IS12" s="0"/>
-      <c r="IT12" s="0"/>
-      <c r="IU12" s="0"/>
-      <c r="IV12" s="0"/>
-      <c r="IW12" s="0"/>
-      <c r="IX12" s="0"/>
-      <c r="IY12" s="0"/>
-      <c r="IZ12" s="0"/>
-      <c r="JA12" s="0"/>
-      <c r="JB12" s="0"/>
-      <c r="JC12" s="0"/>
-      <c r="JD12" s="0"/>
-      <c r="JE12" s="0"/>
-      <c r="JF12" s="0"/>
-      <c r="JG12" s="0"/>
-      <c r="JH12" s="0"/>
-      <c r="JI12" s="0"/>
-      <c r="JJ12" s="0"/>
-      <c r="JK12" s="0"/>
-      <c r="JL12" s="0"/>
-      <c r="JM12" s="0"/>
-      <c r="JN12" s="0"/>
-      <c r="JO12" s="0"/>
-      <c r="JP12" s="0"/>
-      <c r="JQ12" s="0"/>
-      <c r="JR12" s="0"/>
-      <c r="JS12" s="0"/>
-      <c r="JT12" s="0"/>
-      <c r="JU12" s="0"/>
-      <c r="JV12" s="0"/>
-      <c r="JW12" s="0"/>
-      <c r="JX12" s="0"/>
-      <c r="JY12" s="0"/>
-      <c r="JZ12" s="0"/>
-      <c r="KA12" s="0"/>
-      <c r="KB12" s="0"/>
-      <c r="KC12" s="0"/>
-      <c r="KD12" s="0"/>
-      <c r="KE12" s="0"/>
-      <c r="KF12" s="0"/>
-      <c r="KG12" s="0"/>
-      <c r="KH12" s="0"/>
-      <c r="KI12" s="0"/>
-      <c r="KJ12" s="0"/>
-      <c r="KK12" s="0"/>
-      <c r="KL12" s="0"/>
-      <c r="KM12" s="0"/>
-      <c r="KN12" s="0"/>
-      <c r="KO12" s="0"/>
-      <c r="KP12" s="0"/>
-      <c r="KQ12" s="0"/>
-      <c r="KR12" s="0"/>
-      <c r="KS12" s="0"/>
-      <c r="KT12" s="0"/>
-      <c r="KU12" s="0"/>
-      <c r="KV12" s="0"/>
-      <c r="KW12" s="0"/>
-      <c r="KX12" s="0"/>
-      <c r="KY12" s="0"/>
-      <c r="KZ12" s="0"/>
-      <c r="LA12" s="0"/>
-      <c r="LB12" s="0"/>
-      <c r="LC12" s="0"/>
-      <c r="LD12" s="0"/>
-      <c r="LE12" s="0"/>
-      <c r="LF12" s="0"/>
-      <c r="LG12" s="0"/>
-      <c r="LH12" s="0"/>
-      <c r="LI12" s="0"/>
-      <c r="LJ12" s="0"/>
-      <c r="LK12" s="0"/>
-      <c r="LL12" s="0"/>
-      <c r="LM12" s="0"/>
-      <c r="LN12" s="0"/>
-      <c r="LO12" s="0"/>
-      <c r="LP12" s="0"/>
-      <c r="LQ12" s="0"/>
-      <c r="LR12" s="0"/>
-      <c r="LS12" s="0"/>
-      <c r="LT12" s="0"/>
-      <c r="LU12" s="0"/>
-      <c r="LV12" s="0"/>
-      <c r="LW12" s="0"/>
-      <c r="LX12" s="0"/>
-      <c r="LY12" s="0"/>
-      <c r="LZ12" s="0"/>
-      <c r="MA12" s="0"/>
-      <c r="MB12" s="0"/>
-      <c r="MC12" s="0"/>
-      <c r="MD12" s="0"/>
-      <c r="ME12" s="0"/>
-      <c r="MF12" s="0"/>
-      <c r="MG12" s="0"/>
-      <c r="MH12" s="0"/>
-      <c r="MI12" s="0"/>
-      <c r="MJ12" s="0"/>
-      <c r="MK12" s="0"/>
-      <c r="ML12" s="0"/>
-      <c r="MM12" s="0"/>
-      <c r="MN12" s="0"/>
-      <c r="MO12" s="0"/>
-      <c r="MP12" s="0"/>
-      <c r="MQ12" s="0"/>
-      <c r="MR12" s="0"/>
-      <c r="MS12" s="0"/>
-      <c r="MT12" s="0"/>
-      <c r="MU12" s="0"/>
-      <c r="MV12" s="0"/>
-      <c r="MW12" s="0"/>
-      <c r="MX12" s="0"/>
-      <c r="MY12" s="0"/>
-      <c r="MZ12" s="0"/>
-      <c r="NA12" s="0"/>
-      <c r="NB12" s="0"/>
-      <c r="NC12" s="0"/>
-      <c r="ND12" s="0"/>
-      <c r="NE12" s="0"/>
-      <c r="NF12" s="0"/>
-      <c r="NG12" s="0"/>
-      <c r="NH12" s="0"/>
-      <c r="NI12" s="0"/>
-      <c r="NJ12" s="0"/>
-      <c r="NK12" s="0"/>
-      <c r="NL12" s="0"/>
-      <c r="NM12" s="0"/>
-      <c r="NN12" s="0"/>
-      <c r="NO12" s="0"/>
-      <c r="NP12" s="0"/>
-      <c r="NQ12" s="0"/>
-      <c r="NR12" s="0"/>
-      <c r="NS12" s="0"/>
-      <c r="NT12" s="0"/>
-      <c r="NU12" s="0"/>
-      <c r="NV12" s="0"/>
-      <c r="NW12" s="0"/>
-      <c r="NX12" s="0"/>
-      <c r="NY12" s="0"/>
-      <c r="NZ12" s="0"/>
-      <c r="OA12" s="0"/>
-      <c r="OB12" s="0"/>
-      <c r="OC12" s="0"/>
-      <c r="OD12" s="0"/>
-      <c r="OE12" s="0"/>
-      <c r="OF12" s="0"/>
-      <c r="OG12" s="0"/>
-      <c r="OH12" s="0"/>
-      <c r="OI12" s="0"/>
-      <c r="OJ12" s="0"/>
-      <c r="OK12" s="0"/>
-      <c r="OL12" s="0"/>
-      <c r="OM12" s="0"/>
-      <c r="ON12" s="0"/>
-      <c r="OO12" s="0"/>
-      <c r="OP12" s="0"/>
-      <c r="OQ12" s="0"/>
-      <c r="OR12" s="0"/>
-      <c r="OS12" s="0"/>
-      <c r="OT12" s="0"/>
-      <c r="OU12" s="0"/>
-      <c r="OV12" s="0"/>
-      <c r="OW12" s="0"/>
-      <c r="OX12" s="0"/>
-      <c r="OY12" s="0"/>
-      <c r="OZ12" s="0"/>
-      <c r="PA12" s="0"/>
-      <c r="PB12" s="0"/>
-      <c r="PC12" s="0"/>
-      <c r="PD12" s="0"/>
-      <c r="PE12" s="0"/>
-      <c r="PF12" s="0"/>
-      <c r="PG12" s="0"/>
-      <c r="PH12" s="0"/>
-      <c r="PI12" s="0"/>
-      <c r="PJ12" s="0"/>
-      <c r="PK12" s="0"/>
-      <c r="PL12" s="0"/>
-      <c r="PM12" s="0"/>
-      <c r="PN12" s="0"/>
-      <c r="PO12" s="0"/>
-      <c r="PP12" s="0"/>
-      <c r="PQ12" s="0"/>
-      <c r="PR12" s="0"/>
-      <c r="PS12" s="0"/>
-      <c r="PT12" s="0"/>
-      <c r="PU12" s="0"/>
-      <c r="PV12" s="0"/>
-      <c r="PW12" s="0"/>
-      <c r="PX12" s="0"/>
-      <c r="PY12" s="0"/>
-      <c r="PZ12" s="0"/>
-      <c r="QA12" s="0"/>
-      <c r="QB12" s="0"/>
-      <c r="QC12" s="0"/>
-      <c r="QD12" s="0"/>
-      <c r="QE12" s="0"/>
-      <c r="QF12" s="0"/>
-      <c r="QG12" s="0"/>
-      <c r="QH12" s="0"/>
-      <c r="QI12" s="0"/>
-      <c r="QJ12" s="0"/>
-      <c r="QK12" s="0"/>
-      <c r="QL12" s="0"/>
-      <c r="QM12" s="0"/>
-      <c r="QN12" s="0"/>
-      <c r="QO12" s="0"/>
-      <c r="QP12" s="0"/>
-      <c r="QQ12" s="0"/>
-      <c r="QR12" s="0"/>
-      <c r="QS12" s="0"/>
-      <c r="QT12" s="0"/>
-      <c r="QU12" s="0"/>
-      <c r="QV12" s="0"/>
-      <c r="QW12" s="0"/>
-      <c r="QX12" s="0"/>
-      <c r="QY12" s="0"/>
-      <c r="QZ12" s="0"/>
-      <c r="RA12" s="0"/>
-      <c r="RB12" s="0"/>
-      <c r="RC12" s="0"/>
-      <c r="RD12" s="0"/>
-      <c r="RE12" s="0"/>
-      <c r="RF12" s="0"/>
-      <c r="RG12" s="0"/>
-      <c r="RH12" s="0"/>
-      <c r="RI12" s="0"/>
-      <c r="RJ12" s="0"/>
-      <c r="RK12" s="0"/>
-      <c r="RL12" s="0"/>
-      <c r="RM12" s="0"/>
-      <c r="RN12" s="0"/>
-      <c r="RO12" s="0"/>
-      <c r="RP12" s="0"/>
-      <c r="RQ12" s="0"/>
-      <c r="RR12" s="0"/>
-      <c r="RS12" s="0"/>
-      <c r="RT12" s="0"/>
-      <c r="RU12" s="0"/>
-      <c r="RV12" s="0"/>
-      <c r="RW12" s="0"/>
-      <c r="RX12" s="0"/>
-      <c r="RY12" s="0"/>
-      <c r="RZ12" s="0"/>
-      <c r="SA12" s="0"/>
-      <c r="SB12" s="0"/>
-      <c r="SC12" s="0"/>
-      <c r="SD12" s="0"/>
-      <c r="SE12" s="0"/>
-      <c r="SF12" s="0"/>
-      <c r="SG12" s="0"/>
-      <c r="SH12" s="0"/>
-      <c r="SI12" s="0"/>
-      <c r="SJ12" s="0"/>
-      <c r="SK12" s="0"/>
-      <c r="SL12" s="0"/>
-      <c r="SM12" s="0"/>
-      <c r="SN12" s="0"/>
-      <c r="SO12" s="0"/>
-      <c r="SP12" s="0"/>
-      <c r="SQ12" s="0"/>
-      <c r="SR12" s="0"/>
-      <c r="SS12" s="0"/>
-      <c r="ST12" s="0"/>
-      <c r="SU12" s="0"/>
-      <c r="SV12" s="0"/>
-      <c r="SW12" s="0"/>
-      <c r="SX12" s="0"/>
-      <c r="SY12" s="0"/>
-      <c r="SZ12" s="0"/>
-      <c r="TA12" s="0"/>
-      <c r="TB12" s="0"/>
-      <c r="TC12" s="0"/>
-      <c r="TD12" s="0"/>
-      <c r="TE12" s="0"/>
-      <c r="TF12" s="0"/>
-      <c r="TG12" s="0"/>
-      <c r="TH12" s="0"/>
-      <c r="TI12" s="0"/>
-      <c r="TJ12" s="0"/>
-      <c r="TK12" s="0"/>
-      <c r="TL12" s="0"/>
-      <c r="TM12" s="0"/>
-      <c r="TN12" s="0"/>
-      <c r="TO12" s="0"/>
-      <c r="TP12" s="0"/>
-      <c r="TQ12" s="0"/>
-      <c r="TR12" s="0"/>
-      <c r="TS12" s="0"/>
-      <c r="TT12" s="0"/>
-      <c r="TU12" s="0"/>
-      <c r="TV12" s="0"/>
-      <c r="TW12" s="0"/>
-      <c r="TX12" s="0"/>
-      <c r="TY12" s="0"/>
-      <c r="TZ12" s="0"/>
-      <c r="UA12" s="0"/>
-      <c r="UB12" s="0"/>
-      <c r="UC12" s="0"/>
-      <c r="UD12" s="0"/>
-      <c r="UE12" s="0"/>
-      <c r="UF12" s="0"/>
-      <c r="UG12" s="0"/>
-      <c r="UH12" s="0"/>
-      <c r="UI12" s="0"/>
-      <c r="UJ12" s="0"/>
-      <c r="UK12" s="0"/>
-      <c r="UL12" s="0"/>
-      <c r="UM12" s="0"/>
-      <c r="UN12" s="0"/>
-      <c r="UO12" s="0"/>
-      <c r="UP12" s="0"/>
-      <c r="UQ12" s="0"/>
-      <c r="UR12" s="0"/>
-      <c r="US12" s="0"/>
-      <c r="UT12" s="0"/>
-      <c r="UU12" s="0"/>
-      <c r="UV12" s="0"/>
-      <c r="UW12" s="0"/>
-      <c r="UX12" s="0"/>
-      <c r="UY12" s="0"/>
-      <c r="UZ12" s="0"/>
-      <c r="VA12" s="0"/>
-      <c r="VB12" s="0"/>
-      <c r="VC12" s="0"/>
-      <c r="VD12" s="0"/>
-      <c r="VE12" s="0"/>
-      <c r="VF12" s="0"/>
-      <c r="VG12" s="0"/>
-      <c r="VH12" s="0"/>
-      <c r="VI12" s="0"/>
-      <c r="VJ12" s="0"/>
-      <c r="VK12" s="0"/>
-      <c r="VL12" s="0"/>
-      <c r="VM12" s="0"/>
-      <c r="VN12" s="0"/>
-      <c r="VO12" s="0"/>
-      <c r="VP12" s="0"/>
-      <c r="VQ12" s="0"/>
-      <c r="VR12" s="0"/>
-      <c r="VS12" s="0"/>
-      <c r="VT12" s="0"/>
-      <c r="VU12" s="0"/>
-      <c r="VV12" s="0"/>
-      <c r="VW12" s="0"/>
-      <c r="VX12" s="0"/>
-      <c r="VY12" s="0"/>
-      <c r="VZ12" s="0"/>
-      <c r="WA12" s="0"/>
-      <c r="WB12" s="0"/>
-      <c r="WC12" s="0"/>
-      <c r="WD12" s="0"/>
-      <c r="WE12" s="0"/>
-      <c r="WF12" s="0"/>
-      <c r="WG12" s="0"/>
-      <c r="WH12" s="0"/>
-      <c r="WI12" s="0"/>
-      <c r="WJ12" s="0"/>
-      <c r="WK12" s="0"/>
-      <c r="WL12" s="0"/>
-      <c r="WM12" s="0"/>
-      <c r="WN12" s="0"/>
-      <c r="WO12" s="0"/>
-      <c r="WP12" s="0"/>
-      <c r="WQ12" s="0"/>
-      <c r="WR12" s="0"/>
-      <c r="WS12" s="0"/>
-      <c r="WT12" s="0"/>
-      <c r="WU12" s="0"/>
-      <c r="WV12" s="0"/>
-      <c r="WW12" s="0"/>
-      <c r="WX12" s="0"/>
-      <c r="WY12" s="0"/>
-      <c r="WZ12" s="0"/>
-      <c r="XA12" s="0"/>
-      <c r="XB12" s="0"/>
-      <c r="XC12" s="0"/>
-      <c r="XD12" s="0"/>
-      <c r="XE12" s="0"/>
-      <c r="XF12" s="0"/>
-      <c r="XG12" s="0"/>
-      <c r="XH12" s="0"/>
-      <c r="XI12" s="0"/>
-      <c r="XJ12" s="0"/>
-      <c r="XK12" s="0"/>
-      <c r="XL12" s="0"/>
-      <c r="XM12" s="0"/>
-      <c r="XN12" s="0"/>
-      <c r="XO12" s="0"/>
-      <c r="XP12" s="0"/>
-      <c r="XQ12" s="0"/>
-      <c r="XR12" s="0"/>
-      <c r="XS12" s="0"/>
-      <c r="XT12" s="0"/>
-      <c r="XU12" s="0"/>
-      <c r="XV12" s="0"/>
-      <c r="XW12" s="0"/>
-      <c r="XX12" s="0"/>
-      <c r="XY12" s="0"/>
-      <c r="XZ12" s="0"/>
-      <c r="YA12" s="0"/>
-      <c r="YB12" s="0"/>
-      <c r="YC12" s="0"/>
-      <c r="YD12" s="0"/>
-      <c r="YE12" s="0"/>
-      <c r="YF12" s="0"/>
-      <c r="YG12" s="0"/>
-      <c r="YH12" s="0"/>
-      <c r="YI12" s="0"/>
-      <c r="YJ12" s="0"/>
-      <c r="YK12" s="0"/>
-      <c r="YL12" s="0"/>
-      <c r="YM12" s="0"/>
-      <c r="YN12" s="0"/>
-      <c r="YO12" s="0"/>
-      <c r="YP12" s="0"/>
-      <c r="YQ12" s="0"/>
-      <c r="YR12" s="0"/>
-      <c r="YS12" s="0"/>
-      <c r="YT12" s="0"/>
-      <c r="YU12" s="0"/>
-      <c r="YV12" s="0"/>
-      <c r="YW12" s="0"/>
-      <c r="YX12" s="0"/>
-      <c r="YY12" s="0"/>
-      <c r="YZ12" s="0"/>
-      <c r="ZA12" s="0"/>
-      <c r="ZB12" s="0"/>
-      <c r="ZC12" s="0"/>
-      <c r="ZD12" s="0"/>
-      <c r="ZE12" s="0"/>
-      <c r="ZF12" s="0"/>
-      <c r="ZG12" s="0"/>
-      <c r="ZH12" s="0"/>
-      <c r="ZI12" s="0"/>
-      <c r="ZJ12" s="0"/>
-      <c r="ZK12" s="0"/>
-      <c r="ZL12" s="0"/>
-      <c r="ZM12" s="0"/>
-      <c r="ZN12" s="0"/>
-      <c r="ZO12" s="0"/>
-      <c r="ZP12" s="0"/>
-      <c r="ZQ12" s="0"/>
-      <c r="ZR12" s="0"/>
-      <c r="ZS12" s="0"/>
-      <c r="ZT12" s="0"/>
-      <c r="ZU12" s="0"/>
-      <c r="ZV12" s="0"/>
-      <c r="ZW12" s="0"/>
-      <c r="ZX12" s="0"/>
-      <c r="ZY12" s="0"/>
-      <c r="ZZ12" s="0"/>
-      <c r="AAA12" s="0"/>
-      <c r="AAB12" s="0"/>
-      <c r="AAC12" s="0"/>
-      <c r="AAD12" s="0"/>
-      <c r="AAE12" s="0"/>
-      <c r="AAF12" s="0"/>
-      <c r="AAG12" s="0"/>
-      <c r="AAH12" s="0"/>
-      <c r="AAI12" s="0"/>
-      <c r="AAJ12" s="0"/>
-      <c r="AAK12" s="0"/>
-      <c r="AAL12" s="0"/>
-      <c r="AAM12" s="0"/>
-      <c r="AAN12" s="0"/>
-      <c r="AAO12" s="0"/>
-      <c r="AAP12" s="0"/>
-      <c r="AAQ12" s="0"/>
-      <c r="AAR12" s="0"/>
-      <c r="AAS12" s="0"/>
-      <c r="AAT12" s="0"/>
-      <c r="AAU12" s="0"/>
-      <c r="AAV12" s="0"/>
-      <c r="AAW12" s="0"/>
-      <c r="AAX12" s="0"/>
-      <c r="AAY12" s="0"/>
-      <c r="AAZ12" s="0"/>
-      <c r="ABA12" s="0"/>
-      <c r="ABB12" s="0"/>
-      <c r="ABC12" s="0"/>
-      <c r="ABD12" s="0"/>
-      <c r="ABE12" s="0"/>
-      <c r="ABF12" s="0"/>
-      <c r="ABG12" s="0"/>
-      <c r="ABH12" s="0"/>
-      <c r="ABI12" s="0"/>
-      <c r="ABJ12" s="0"/>
-      <c r="ABK12" s="0"/>
-      <c r="ABL12" s="0"/>
-      <c r="ABM12" s="0"/>
-      <c r="ABN12" s="0"/>
-      <c r="ABO12" s="0"/>
-      <c r="ABP12" s="0"/>
-      <c r="ABQ12" s="0"/>
-      <c r="ABR12" s="0"/>
-      <c r="ABS12" s="0"/>
-      <c r="ABT12" s="0"/>
-      <c r="ABU12" s="0"/>
-      <c r="ABV12" s="0"/>
-      <c r="ABW12" s="0"/>
-      <c r="ABX12" s="0"/>
-      <c r="ABY12" s="0"/>
-      <c r="ABZ12" s="0"/>
-      <c r="ACA12" s="0"/>
-      <c r="ACB12" s="0"/>
-      <c r="ACC12" s="0"/>
-      <c r="ACD12" s="0"/>
-      <c r="ACE12" s="0"/>
-      <c r="ACF12" s="0"/>
-      <c r="ACG12" s="0"/>
-      <c r="ACH12" s="0"/>
-      <c r="ACI12" s="0"/>
-      <c r="ACJ12" s="0"/>
-      <c r="ACK12" s="0"/>
-      <c r="ACL12" s="0"/>
-      <c r="ACM12" s="0"/>
-      <c r="ACN12" s="0"/>
-      <c r="ACO12" s="0"/>
-      <c r="ACP12" s="0"/>
-      <c r="ACQ12" s="0"/>
-      <c r="ACR12" s="0"/>
-      <c r="ACS12" s="0"/>
-      <c r="ACT12" s="0"/>
-      <c r="ACU12" s="0"/>
-      <c r="ACV12" s="0"/>
-      <c r="ACW12" s="0"/>
-      <c r="ACX12" s="0"/>
-      <c r="ACY12" s="0"/>
-      <c r="ACZ12" s="0"/>
-      <c r="ADA12" s="0"/>
-      <c r="ADB12" s="0"/>
-      <c r="ADC12" s="0"/>
-      <c r="ADD12" s="0"/>
-      <c r="ADE12" s="0"/>
-      <c r="ADF12" s="0"/>
-      <c r="ADG12" s="0"/>
-      <c r="ADH12" s="0"/>
-      <c r="ADI12" s="0"/>
-      <c r="ADJ12" s="0"/>
-      <c r="ADK12" s="0"/>
-      <c r="ADL12" s="0"/>
-      <c r="ADM12" s="0"/>
-      <c r="ADN12" s="0"/>
-      <c r="ADO12" s="0"/>
-      <c r="ADP12" s="0"/>
-      <c r="ADQ12" s="0"/>
-      <c r="ADR12" s="0"/>
-      <c r="ADS12" s="0"/>
-      <c r="ADT12" s="0"/>
-      <c r="ADU12" s="0"/>
-      <c r="ADV12" s="0"/>
-      <c r="ADW12" s="0"/>
-      <c r="ADX12" s="0"/>
-      <c r="ADY12" s="0"/>
-      <c r="ADZ12" s="0"/>
-      <c r="AEA12" s="0"/>
-      <c r="AEB12" s="0"/>
-      <c r="AEC12" s="0"/>
-      <c r="AED12" s="0"/>
-      <c r="AEE12" s="0"/>
-      <c r="AEF12" s="0"/>
-      <c r="AEG12" s="0"/>
-      <c r="AEH12" s="0"/>
-      <c r="AEI12" s="0"/>
-      <c r="AEJ12" s="0"/>
-      <c r="AEK12" s="0"/>
-      <c r="AEL12" s="0"/>
-      <c r="AEM12" s="0"/>
-      <c r="AEN12" s="0"/>
-      <c r="AEO12" s="0"/>
-      <c r="AEP12" s="0"/>
-      <c r="AEQ12" s="0"/>
-      <c r="AER12" s="0"/>
-      <c r="AES12" s="0"/>
-      <c r="AET12" s="0"/>
-      <c r="AEU12" s="0"/>
-      <c r="AEV12" s="0"/>
-      <c r="AEW12" s="0"/>
-      <c r="AEX12" s="0"/>
-      <c r="AEY12" s="0"/>
-      <c r="AEZ12" s="0"/>
-      <c r="AFA12" s="0"/>
-      <c r="AFB12" s="0"/>
-      <c r="AFC12" s="0"/>
-      <c r="AFD12" s="0"/>
-      <c r="AFE12" s="0"/>
-      <c r="AFF12" s="0"/>
-      <c r="AFG12" s="0"/>
-      <c r="AFH12" s="0"/>
-      <c r="AFI12" s="0"/>
-      <c r="AFJ12" s="0"/>
-      <c r="AFK12" s="0"/>
-      <c r="AFL12" s="0"/>
-      <c r="AFM12" s="0"/>
-      <c r="AFN12" s="0"/>
-      <c r="AFO12" s="0"/>
-      <c r="AFP12" s="0"/>
-      <c r="AFQ12" s="0"/>
-      <c r="AFR12" s="0"/>
-      <c r="AFS12" s="0"/>
-      <c r="AFT12" s="0"/>
-      <c r="AFU12" s="0"/>
-      <c r="AFV12" s="0"/>
-      <c r="AFW12" s="0"/>
-      <c r="AFX12" s="0"/>
-      <c r="AFY12" s="0"/>
-      <c r="AFZ12" s="0"/>
-      <c r="AGA12" s="0"/>
-      <c r="AGB12" s="0"/>
-      <c r="AGC12" s="0"/>
-      <c r="AGD12" s="0"/>
-      <c r="AGE12" s="0"/>
-      <c r="AGF12" s="0"/>
-      <c r="AGG12" s="0"/>
-      <c r="AGH12" s="0"/>
-      <c r="AGI12" s="0"/>
-      <c r="AGJ12" s="0"/>
-      <c r="AGK12" s="0"/>
-      <c r="AGL12" s="0"/>
-      <c r="AGM12" s="0"/>
-      <c r="AGN12" s="0"/>
-      <c r="AGO12" s="0"/>
-      <c r="AGP12" s="0"/>
-      <c r="AGQ12" s="0"/>
-      <c r="AGR12" s="0"/>
-      <c r="AGS12" s="0"/>
-      <c r="AGT12" s="0"/>
-      <c r="AGU12" s="0"/>
-      <c r="AGV12" s="0"/>
-      <c r="AGW12" s="0"/>
-      <c r="AGX12" s="0"/>
-      <c r="AGY12" s="0"/>
-      <c r="AGZ12" s="0"/>
-      <c r="AHA12" s="0"/>
-      <c r="AHB12" s="0"/>
-      <c r="AHC12" s="0"/>
-      <c r="AHD12" s="0"/>
-      <c r="AHE12" s="0"/>
-      <c r="AHF12" s="0"/>
-      <c r="AHG12" s="0"/>
-      <c r="AHH12" s="0"/>
-      <c r="AHI12" s="0"/>
-      <c r="AHJ12" s="0"/>
-      <c r="AHK12" s="0"/>
-      <c r="AHL12" s="0"/>
-      <c r="AHM12" s="0"/>
-      <c r="AHN12" s="0"/>
-      <c r="AHO12" s="0"/>
-      <c r="AHP12" s="0"/>
-      <c r="AHQ12" s="0"/>
-      <c r="AHR12" s="0"/>
-      <c r="AHS12" s="0"/>
-      <c r="AHT12" s="0"/>
-      <c r="AHU12" s="0"/>
-      <c r="AHV12" s="0"/>
-      <c r="AHW12" s="0"/>
-      <c r="AHX12" s="0"/>
-      <c r="AHY12" s="0"/>
-      <c r="AHZ12" s="0"/>
-      <c r="AIA12" s="0"/>
-      <c r="AIB12" s="0"/>
-      <c r="AIC12" s="0"/>
-      <c r="AID12" s="0"/>
-      <c r="AIE12" s="0"/>
-      <c r="AIF12" s="0"/>
-      <c r="AIG12" s="0"/>
-      <c r="AIH12" s="0"/>
-      <c r="AII12" s="0"/>
-      <c r="AIJ12" s="0"/>
-      <c r="AIK12" s="0"/>
-      <c r="AIL12" s="0"/>
-      <c r="AIM12" s="0"/>
-      <c r="AIN12" s="0"/>
-      <c r="AIO12" s="0"/>
-      <c r="AIP12" s="0"/>
-      <c r="AIQ12" s="0"/>
-      <c r="AIR12" s="0"/>
-      <c r="AIS12" s="0"/>
-      <c r="AIT12" s="0"/>
-      <c r="AIU12" s="0"/>
-      <c r="AIV12" s="0"/>
-      <c r="AIW12" s="0"/>
-      <c r="AIX12" s="0"/>
-      <c r="AIY12" s="0"/>
-      <c r="AIZ12" s="0"/>
-      <c r="AJA12" s="0"/>
-      <c r="AJB12" s="0"/>
-      <c r="AJC12" s="0"/>
-      <c r="AJD12" s="0"/>
-      <c r="AJE12" s="0"/>
-      <c r="AJF12" s="0"/>
-      <c r="AJG12" s="0"/>
-      <c r="AJH12" s="0"/>
-      <c r="AJI12" s="0"/>
-      <c r="AJJ12" s="0"/>
-      <c r="AJK12" s="0"/>
-      <c r="AJL12" s="0"/>
-      <c r="AJM12" s="0"/>
-      <c r="AJN12" s="0"/>
-      <c r="AJO12" s="0"/>
-      <c r="AJP12" s="0"/>
-      <c r="AJQ12" s="0"/>
-      <c r="AJR12" s="0"/>
-      <c r="AJS12" s="0"/>
-      <c r="AJT12" s="0"/>
-      <c r="AJU12" s="0"/>
-      <c r="AJV12" s="0"/>
-      <c r="AJW12" s="0"/>
-      <c r="AJX12" s="0"/>
-      <c r="AJY12" s="0"/>
-      <c r="AJZ12" s="0"/>
-      <c r="AKA12" s="0"/>
-      <c r="AKB12" s="0"/>
-      <c r="AKC12" s="0"/>
-      <c r="AKD12" s="0"/>
-      <c r="AKE12" s="0"/>
-      <c r="AKF12" s="0"/>
-      <c r="AKG12" s="0"/>
-      <c r="AKH12" s="0"/>
-      <c r="AKI12" s="0"/>
-      <c r="AKJ12" s="0"/>
-      <c r="AKK12" s="0"/>
-      <c r="AKL12" s="0"/>
-      <c r="AKM12" s="0"/>
-      <c r="AKN12" s="0"/>
-      <c r="AKO12" s="0"/>
-      <c r="AKP12" s="0"/>
-      <c r="AKQ12" s="0"/>
-      <c r="AKR12" s="0"/>
-      <c r="AKS12" s="0"/>
-      <c r="AKT12" s="0"/>
-      <c r="AKU12" s="0"/>
-      <c r="AKV12" s="0"/>
-      <c r="AKW12" s="0"/>
-      <c r="AKX12" s="0"/>
-      <c r="AKY12" s="0"/>
-      <c r="AKZ12" s="0"/>
-      <c r="ALA12" s="0"/>
-      <c r="ALB12" s="0"/>
-      <c r="ALC12" s="0"/>
-      <c r="ALD12" s="0"/>
-      <c r="ALE12" s="0"/>
-      <c r="ALF12" s="0"/>
-      <c r="ALG12" s="0"/>
-      <c r="ALH12" s="0"/>
-      <c r="ALI12" s="0"/>
-      <c r="ALJ12" s="0"/>
-      <c r="ALK12" s="0"/>
-      <c r="ALL12" s="0"/>
-      <c r="ALM12" s="0"/>
-      <c r="ALN12" s="0"/>
-      <c r="ALO12" s="0"/>
-      <c r="ALP12" s="0"/>
-      <c r="ALQ12" s="0"/>
-      <c r="ALR12" s="0"/>
-      <c r="ALS12" s="0"/>
-      <c r="ALT12" s="0"/>
-      <c r="ALU12" s="0"/>
-      <c r="ALV12" s="0"/>
-      <c r="ALW12" s="0"/>
-      <c r="ALX12" s="0"/>
-      <c r="ALY12" s="0"/>
-      <c r="ALZ12" s="0"/>
-      <c r="AMA12" s="0"/>
-      <c r="AMB12" s="0"/>
-      <c r="AMC12" s="0"/>
-      <c r="AMD12" s="0"/>
-    </row>
-    <row r="13" s="20" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="G13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="H13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="18" t="s">
+    </row>
+    <row r="14" s="16" customFormat="true" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="E14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="19" t="e">
-        <f aca="true">INDIRECT( "F" &amp; ROW() )+INDIRECT( "G" &amp; ROW() )</f>
-        <v>#VALUE!</v>
+      <c r="F14" s="13" t="s">
+        <v>21</v>
       </c>
-      <c r="AME13" s="0"/>
-      <c r="AMF13" s="0"/>
-      <c r="AMG13" s="0"/>
-      <c r="AMH13" s="0"/>
-      <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
+      <c r="G14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AME14" s="14"/>
+      <c r="AMF14" s="14"/>
+      <c r="AMG14" s="14"/>
+      <c r="AMH14" s="14"/>
+      <c r="AMI14" s="14"/>
+      <c r="AMJ14" s="14"/>
     </row>
-    <row r="14" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13" t="s">
+    <row r="15" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="15" t="e">
-        <f aca="true">INDIRECT( "G" &amp; ROW() )+INDIRECT( "F" &amp; ROW() )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I14" s="0"/>
-      <c r="J14" s="0"/>
-      <c r="K14" s="0"/>
-      <c r="L14" s="0"/>
-      <c r="M14" s="0"/>
-      <c r="N14" s="0"/>
-      <c r="O14" s="0"/>
-      <c r="P14" s="0"/>
-      <c r="Q14" s="0"/>
-      <c r="R14" s="0"/>
-      <c r="S14" s="0"/>
-      <c r="T14" s="0"/>
-      <c r="U14" s="0"/>
-      <c r="V14" s="0"/>
-      <c r="W14" s="0"/>
-      <c r="X14" s="0"/>
-      <c r="Y14" s="0"/>
-      <c r="Z14" s="0"/>
-      <c r="AA14" s="0"/>
-      <c r="AB14" s="0"/>
-      <c r="AC14" s="0"/>
-      <c r="AD14" s="0"/>
-      <c r="AE14" s="0"/>
-      <c r="AF14" s="0"/>
-      <c r="AG14" s="0"/>
-      <c r="AH14" s="0"/>
-      <c r="AI14" s="0"/>
-      <c r="AJ14" s="0"/>
-      <c r="AK14" s="0"/>
-      <c r="AL14" s="0"/>
-      <c r="AM14" s="0"/>
-      <c r="AN14" s="0"/>
-      <c r="AO14" s="0"/>
-      <c r="AP14" s="0"/>
-      <c r="AQ14" s="0"/>
-      <c r="AR14" s="0"/>
-      <c r="AS14" s="0"/>
-      <c r="AT14" s="0"/>
-      <c r="AU14" s="0"/>
-      <c r="AV14" s="0"/>
-      <c r="AW14" s="0"/>
-      <c r="AX14" s="0"/>
-      <c r="AY14" s="0"/>
-      <c r="AZ14" s="0"/>
-      <c r="BA14" s="0"/>
-      <c r="BB14" s="0"/>
-      <c r="BC14" s="0"/>
-      <c r="BD14" s="0"/>
-      <c r="BE14" s="0"/>
-      <c r="BF14" s="0"/>
-      <c r="BG14" s="0"/>
-      <c r="BH14" s="0"/>
-      <c r="BI14" s="0"/>
-      <c r="BJ14" s="0"/>
-      <c r="BK14" s="0"/>
-      <c r="BL14" s="0"/>
-      <c r="BM14" s="0"/>
-      <c r="BN14" s="0"/>
-      <c r="BO14" s="0"/>
-      <c r="BP14" s="0"/>
-      <c r="BQ14" s="0"/>
-      <c r="BR14" s="0"/>
-      <c r="BS14" s="0"/>
-      <c r="BT14" s="0"/>
-      <c r="BU14" s="0"/>
-      <c r="BV14" s="0"/>
-      <c r="BW14" s="0"/>
-      <c r="BX14" s="0"/>
-      <c r="BY14" s="0"/>
-      <c r="BZ14" s="0"/>
-      <c r="CA14" s="0"/>
-      <c r="CB14" s="0"/>
-      <c r="CC14" s="0"/>
-      <c r="CD14" s="0"/>
-      <c r="CE14" s="0"/>
-      <c r="CF14" s="0"/>
-      <c r="CG14" s="0"/>
-      <c r="CH14" s="0"/>
-      <c r="CI14" s="0"/>
-      <c r="CJ14" s="0"/>
-      <c r="CK14" s="0"/>
-      <c r="CL14" s="0"/>
-      <c r="CM14" s="0"/>
-      <c r="CN14" s="0"/>
-      <c r="CO14" s="0"/>
-      <c r="CP14" s="0"/>
-      <c r="CQ14" s="0"/>
-      <c r="CR14" s="0"/>
-      <c r="CS14" s="0"/>
-      <c r="CT14" s="0"/>
-      <c r="CU14" s="0"/>
-      <c r="CV14" s="0"/>
-      <c r="CW14" s="0"/>
-      <c r="CX14" s="0"/>
-      <c r="CY14" s="0"/>
-      <c r="CZ14" s="0"/>
-      <c r="DA14" s="0"/>
-      <c r="DB14" s="0"/>
-      <c r="DC14" s="0"/>
-      <c r="DD14" s="0"/>
-      <c r="DE14" s="0"/>
-      <c r="DF14" s="0"/>
-      <c r="DG14" s="0"/>
-      <c r="DH14" s="0"/>
-      <c r="DI14" s="0"/>
-      <c r="DJ14" s="0"/>
-      <c r="DK14" s="0"/>
-      <c r="DL14" s="0"/>
-      <c r="DM14" s="0"/>
-      <c r="DN14" s="0"/>
-      <c r="DO14" s="0"/>
-      <c r="DP14" s="0"/>
-      <c r="DQ14" s="0"/>
-      <c r="DR14" s="0"/>
-      <c r="DS14" s="0"/>
-      <c r="DT14" s="0"/>
-      <c r="DU14" s="0"/>
-      <c r="DV14" s="0"/>
-      <c r="DW14" s="0"/>
-      <c r="DX14" s="0"/>
-      <c r="DY14" s="0"/>
-      <c r="DZ14" s="0"/>
-      <c r="EA14" s="0"/>
-      <c r="EB14" s="0"/>
-      <c r="EC14" s="0"/>
-      <c r="ED14" s="0"/>
-      <c r="EE14" s="0"/>
-      <c r="EF14" s="0"/>
-      <c r="EG14" s="0"/>
-      <c r="EH14" s="0"/>
-      <c r="EI14" s="0"/>
-      <c r="EJ14" s="0"/>
-      <c r="EK14" s="0"/>
-      <c r="EL14" s="0"/>
-      <c r="EM14" s="0"/>
-      <c r="EN14" s="0"/>
-      <c r="EO14" s="0"/>
-      <c r="EP14" s="0"/>
-      <c r="EQ14" s="0"/>
-      <c r="ER14" s="0"/>
-      <c r="ES14" s="0"/>
-      <c r="ET14" s="0"/>
-      <c r="EU14" s="0"/>
-      <c r="EV14" s="0"/>
-      <c r="EW14" s="0"/>
-      <c r="EX14" s="0"/>
-      <c r="EY14" s="0"/>
-      <c r="EZ14" s="0"/>
-      <c r="FA14" s="0"/>
-      <c r="FB14" s="0"/>
-      <c r="FC14" s="0"/>
-      <c r="FD14" s="0"/>
-      <c r="FE14" s="0"/>
-      <c r="FF14" s="0"/>
-      <c r="FG14" s="0"/>
-      <c r="FH14" s="0"/>
-      <c r="FI14" s="0"/>
-      <c r="FJ14" s="0"/>
-      <c r="FK14" s="0"/>
-      <c r="FL14" s="0"/>
-      <c r="FM14" s="0"/>
-      <c r="FN14" s="0"/>
-      <c r="FO14" s="0"/>
-      <c r="FP14" s="0"/>
-      <c r="FQ14" s="0"/>
-      <c r="FR14" s="0"/>
-      <c r="FS14" s="0"/>
-      <c r="FT14" s="0"/>
-      <c r="FU14" s="0"/>
-      <c r="FV14" s="0"/>
-      <c r="FW14" s="0"/>
-      <c r="FX14" s="0"/>
-      <c r="FY14" s="0"/>
-      <c r="FZ14" s="0"/>
-      <c r="GA14" s="0"/>
-      <c r="GB14" s="0"/>
-      <c r="GC14" s="0"/>
-      <c r="GD14" s="0"/>
-      <c r="GE14" s="0"/>
-      <c r="GF14" s="0"/>
-      <c r="GG14" s="0"/>
-      <c r="GH14" s="0"/>
-      <c r="GI14" s="0"/>
-      <c r="GJ14" s="0"/>
-      <c r="GK14" s="0"/>
-      <c r="GL14" s="0"/>
-      <c r="GM14" s="0"/>
-      <c r="GN14" s="0"/>
-      <c r="GO14" s="0"/>
-      <c r="GP14" s="0"/>
-      <c r="GQ14" s="0"/>
-      <c r="GR14" s="0"/>
-      <c r="GS14" s="0"/>
-      <c r="GT14" s="0"/>
-      <c r="GU14" s="0"/>
-      <c r="GV14" s="0"/>
-      <c r="GW14" s="0"/>
-      <c r="GX14" s="0"/>
-      <c r="GY14" s="0"/>
-      <c r="GZ14" s="0"/>
-      <c r="HA14" s="0"/>
-      <c r="HB14" s="0"/>
-      <c r="HC14" s="0"/>
-      <c r="HD14" s="0"/>
-      <c r="HE14" s="0"/>
-      <c r="HF14" s="0"/>
-      <c r="HG14" s="0"/>
-      <c r="HH14" s="0"/>
-      <c r="HI14" s="0"/>
-      <c r="HJ14" s="0"/>
-      <c r="HK14" s="0"/>
-      <c r="HL14" s="0"/>
-      <c r="HM14" s="0"/>
-      <c r="HN14" s="0"/>
-      <c r="HO14" s="0"/>
-      <c r="HP14" s="0"/>
-      <c r="HQ14" s="0"/>
-      <c r="HR14" s="0"/>
-      <c r="HS14" s="0"/>
-      <c r="HT14" s="0"/>
-      <c r="HU14" s="0"/>
-      <c r="HV14" s="0"/>
-      <c r="HW14" s="0"/>
-      <c r="HX14" s="0"/>
-      <c r="HY14" s="0"/>
-      <c r="HZ14" s="0"/>
-      <c r="IA14" s="0"/>
-      <c r="IB14" s="0"/>
-      <c r="IC14" s="0"/>
-      <c r="ID14" s="0"/>
-      <c r="IE14" s="0"/>
-      <c r="IF14" s="0"/>
-      <c r="IG14" s="0"/>
-      <c r="IH14" s="0"/>
-      <c r="II14" s="0"/>
-      <c r="IJ14" s="0"/>
-      <c r="IK14" s="0"/>
-      <c r="IL14" s="0"/>
-      <c r="IM14" s="0"/>
-      <c r="IN14" s="0"/>
-      <c r="IO14" s="0"/>
-      <c r="IP14" s="0"/>
-      <c r="IQ14" s="0"/>
-      <c r="IR14" s="0"/>
-      <c r="IS14" s="0"/>
-      <c r="IT14" s="0"/>
-      <c r="IU14" s="0"/>
-      <c r="IV14" s="0"/>
-      <c r="IW14" s="0"/>
-      <c r="IX14" s="0"/>
-      <c r="IY14" s="0"/>
-      <c r="IZ14" s="0"/>
-      <c r="JA14" s="0"/>
-      <c r="JB14" s="0"/>
-      <c r="JC14" s="0"/>
-      <c r="JD14" s="0"/>
-      <c r="JE14" s="0"/>
-      <c r="JF14" s="0"/>
-      <c r="JG14" s="0"/>
-      <c r="JH14" s="0"/>
-      <c r="JI14" s="0"/>
-      <c r="JJ14" s="0"/>
-      <c r="JK14" s="0"/>
-      <c r="JL14" s="0"/>
-      <c r="JM14" s="0"/>
-      <c r="JN14" s="0"/>
-      <c r="JO14" s="0"/>
-      <c r="JP14" s="0"/>
-      <c r="JQ14" s="0"/>
-      <c r="JR14" s="0"/>
-      <c r="JS14" s="0"/>
-      <c r="JT14" s="0"/>
-      <c r="JU14" s="0"/>
-      <c r="JV14" s="0"/>
-      <c r="JW14" s="0"/>
-      <c r="JX14" s="0"/>
-      <c r="JY14" s="0"/>
-      <c r="JZ14" s="0"/>
-      <c r="KA14" s="0"/>
-      <c r="KB14" s="0"/>
-      <c r="KC14" s="0"/>
-      <c r="KD14" s="0"/>
-      <c r="KE14" s="0"/>
-      <c r="KF14" s="0"/>
-      <c r="KG14" s="0"/>
-      <c r="KH14" s="0"/>
-      <c r="KI14" s="0"/>
-      <c r="KJ14" s="0"/>
-      <c r="KK14" s="0"/>
-      <c r="KL14" s="0"/>
-      <c r="KM14" s="0"/>
-      <c r="KN14" s="0"/>
-      <c r="KO14" s="0"/>
-      <c r="KP14" s="0"/>
-      <c r="KQ14" s="0"/>
-      <c r="KR14" s="0"/>
-      <c r="KS14" s="0"/>
-      <c r="KT14" s="0"/>
-      <c r="KU14" s="0"/>
-      <c r="KV14" s="0"/>
-      <c r="KW14" s="0"/>
-      <c r="KX14" s="0"/>
-      <c r="KY14" s="0"/>
-      <c r="KZ14" s="0"/>
-      <c r="LA14" s="0"/>
-      <c r="LB14" s="0"/>
-      <c r="LC14" s="0"/>
-      <c r="LD14" s="0"/>
-      <c r="LE14" s="0"/>
-      <c r="LF14" s="0"/>
-      <c r="LG14" s="0"/>
-      <c r="LH14" s="0"/>
-      <c r="LI14" s="0"/>
-      <c r="LJ14" s="0"/>
-      <c r="LK14" s="0"/>
-      <c r="LL14" s="0"/>
-      <c r="LM14" s="0"/>
-      <c r="LN14" s="0"/>
-      <c r="LO14" s="0"/>
-      <c r="LP14" s="0"/>
-      <c r="LQ14" s="0"/>
-      <c r="LR14" s="0"/>
-      <c r="LS14" s="0"/>
-      <c r="LT14" s="0"/>
-      <c r="LU14" s="0"/>
-      <c r="LV14" s="0"/>
-      <c r="LW14" s="0"/>
-      <c r="LX14" s="0"/>
-      <c r="LY14" s="0"/>
-      <c r="LZ14" s="0"/>
-      <c r="MA14" s="0"/>
-      <c r="MB14" s="0"/>
-      <c r="MC14" s="0"/>
-      <c r="MD14" s="0"/>
-      <c r="ME14" s="0"/>
-      <c r="MF14" s="0"/>
-      <c r="MG14" s="0"/>
-      <c r="MH14" s="0"/>
-      <c r="MI14" s="0"/>
-      <c r="MJ14" s="0"/>
-      <c r="MK14" s="0"/>
-      <c r="ML14" s="0"/>
-      <c r="MM14" s="0"/>
-      <c r="MN14" s="0"/>
-      <c r="MO14" s="0"/>
-      <c r="MP14" s="0"/>
-      <c r="MQ14" s="0"/>
-      <c r="MR14" s="0"/>
-      <c r="MS14" s="0"/>
-      <c r="MT14" s="0"/>
-      <c r="MU14" s="0"/>
-      <c r="MV14" s="0"/>
-      <c r="MW14" s="0"/>
-      <c r="MX14" s="0"/>
-      <c r="MY14" s="0"/>
-      <c r="MZ14" s="0"/>
-      <c r="NA14" s="0"/>
-      <c r="NB14" s="0"/>
-      <c r="NC14" s="0"/>
-      <c r="ND14" s="0"/>
-      <c r="NE14" s="0"/>
-      <c r="NF14" s="0"/>
-      <c r="NG14" s="0"/>
-      <c r="NH14" s="0"/>
-      <c r="NI14" s="0"/>
-      <c r="NJ14" s="0"/>
-      <c r="NK14" s="0"/>
-      <c r="NL14" s="0"/>
-      <c r="NM14" s="0"/>
-      <c r="NN14" s="0"/>
-      <c r="NO14" s="0"/>
-      <c r="NP14" s="0"/>
-      <c r="NQ14" s="0"/>
-      <c r="NR14" s="0"/>
-      <c r="NS14" s="0"/>
-      <c r="NT14" s="0"/>
-      <c r="NU14" s="0"/>
-      <c r="NV14" s="0"/>
-      <c r="NW14" s="0"/>
-      <c r="NX14" s="0"/>
-      <c r="NY14" s="0"/>
-      <c r="NZ14" s="0"/>
-      <c r="OA14" s="0"/>
-      <c r="OB14" s="0"/>
-      <c r="OC14" s="0"/>
-      <c r="OD14" s="0"/>
-      <c r="OE14" s="0"/>
-      <c r="OF14" s="0"/>
-      <c r="OG14" s="0"/>
-      <c r="OH14" s="0"/>
-      <c r="OI14" s="0"/>
-      <c r="OJ14" s="0"/>
-      <c r="OK14" s="0"/>
-      <c r="OL14" s="0"/>
-      <c r="OM14" s="0"/>
-      <c r="ON14" s="0"/>
-      <c r="OO14" s="0"/>
-      <c r="OP14" s="0"/>
-      <c r="OQ14" s="0"/>
-      <c r="OR14" s="0"/>
-      <c r="OS14" s="0"/>
-      <c r="OT14" s="0"/>
-      <c r="OU14" s="0"/>
-      <c r="OV14" s="0"/>
-      <c r="OW14" s="0"/>
-      <c r="OX14" s="0"/>
-      <c r="OY14" s="0"/>
-      <c r="OZ14" s="0"/>
-      <c r="PA14" s="0"/>
-      <c r="PB14" s="0"/>
-      <c r="PC14" s="0"/>
-      <c r="PD14" s="0"/>
-      <c r="PE14" s="0"/>
-      <c r="PF14" s="0"/>
-      <c r="PG14" s="0"/>
-      <c r="PH14" s="0"/>
-      <c r="PI14" s="0"/>
-      <c r="PJ14" s="0"/>
-      <c r="PK14" s="0"/>
-      <c r="PL14" s="0"/>
-      <c r="PM14" s="0"/>
-      <c r="PN14" s="0"/>
-      <c r="PO14" s="0"/>
-      <c r="PP14" s="0"/>
-      <c r="PQ14" s="0"/>
-      <c r="PR14" s="0"/>
-      <c r="PS14" s="0"/>
-      <c r="PT14" s="0"/>
-      <c r="PU14" s="0"/>
-      <c r="PV14" s="0"/>
-      <c r="PW14" s="0"/>
-      <c r="PX14" s="0"/>
-      <c r="PY14" s="0"/>
-      <c r="PZ14" s="0"/>
-      <c r="QA14" s="0"/>
-      <c r="QB14" s="0"/>
-      <c r="QC14" s="0"/>
-      <c r="QD14" s="0"/>
-      <c r="QE14" s="0"/>
-      <c r="QF14" s="0"/>
-      <c r="QG14" s="0"/>
-      <c r="QH14" s="0"/>
-      <c r="QI14" s="0"/>
-      <c r="QJ14" s="0"/>
-      <c r="QK14" s="0"/>
-      <c r="QL14" s="0"/>
-      <c r="QM14" s="0"/>
-      <c r="QN14" s="0"/>
-      <c r="QO14" s="0"/>
-      <c r="QP14" s="0"/>
-      <c r="QQ14" s="0"/>
-      <c r="QR14" s="0"/>
-      <c r="QS14" s="0"/>
-      <c r="QT14" s="0"/>
-      <c r="QU14" s="0"/>
-      <c r="QV14" s="0"/>
-      <c r="QW14" s="0"/>
-      <c r="QX14" s="0"/>
-      <c r="QY14" s="0"/>
-      <c r="QZ14" s="0"/>
-      <c r="RA14" s="0"/>
-      <c r="RB14" s="0"/>
-      <c r="RC14" s="0"/>
-      <c r="RD14" s="0"/>
-      <c r="RE14" s="0"/>
-      <c r="RF14" s="0"/>
-      <c r="RG14" s="0"/>
-      <c r="RH14" s="0"/>
-      <c r="RI14" s="0"/>
-      <c r="RJ14" s="0"/>
-      <c r="RK14" s="0"/>
-      <c r="RL14" s="0"/>
-      <c r="RM14" s="0"/>
-      <c r="RN14" s="0"/>
-      <c r="RO14" s="0"/>
-      <c r="RP14" s="0"/>
-      <c r="RQ14" s="0"/>
-      <c r="RR14" s="0"/>
-      <c r="RS14" s="0"/>
-      <c r="RT14" s="0"/>
-      <c r="RU14" s="0"/>
-      <c r="RV14" s="0"/>
-      <c r="RW14" s="0"/>
-      <c r="RX14" s="0"/>
-      <c r="RY14" s="0"/>
-      <c r="RZ14" s="0"/>
-      <c r="SA14" s="0"/>
-      <c r="SB14" s="0"/>
-      <c r="SC14" s="0"/>
-      <c r="SD14" s="0"/>
-      <c r="SE14" s="0"/>
-      <c r="SF14" s="0"/>
-      <c r="SG14" s="0"/>
-      <c r="SH14" s="0"/>
-      <c r="SI14" s="0"/>
-      <c r="SJ14" s="0"/>
-      <c r="SK14" s="0"/>
-      <c r="SL14" s="0"/>
-      <c r="SM14" s="0"/>
-      <c r="SN14" s="0"/>
-      <c r="SO14" s="0"/>
-      <c r="SP14" s="0"/>
-      <c r="SQ14" s="0"/>
-      <c r="SR14" s="0"/>
-      <c r="SS14" s="0"/>
-      <c r="ST14" s="0"/>
-      <c r="SU14" s="0"/>
-      <c r="SV14" s="0"/>
-      <c r="SW14" s="0"/>
-      <c r="SX14" s="0"/>
-      <c r="SY14" s="0"/>
-      <c r="SZ14" s="0"/>
-      <c r="TA14" s="0"/>
-      <c r="TB14" s="0"/>
-      <c r="TC14" s="0"/>
-      <c r="TD14" s="0"/>
-      <c r="TE14" s="0"/>
-      <c r="TF14" s="0"/>
-      <c r="TG14" s="0"/>
-      <c r="TH14" s="0"/>
-      <c r="TI14" s="0"/>
-      <c r="TJ14" s="0"/>
-      <c r="TK14" s="0"/>
-      <c r="TL14" s="0"/>
-      <c r="TM14" s="0"/>
-      <c r="TN14" s="0"/>
-      <c r="TO14" s="0"/>
-      <c r="TP14" s="0"/>
-      <c r="TQ14" s="0"/>
-      <c r="TR14" s="0"/>
-      <c r="TS14" s="0"/>
-      <c r="TT14" s="0"/>
-      <c r="TU14" s="0"/>
-      <c r="TV14" s="0"/>
-      <c r="TW14" s="0"/>
-      <c r="TX14" s="0"/>
-      <c r="TY14" s="0"/>
-      <c r="TZ14" s="0"/>
-      <c r="UA14" s="0"/>
-      <c r="UB14" s="0"/>
-      <c r="UC14" s="0"/>
-      <c r="UD14" s="0"/>
-      <c r="UE14" s="0"/>
-      <c r="UF14" s="0"/>
-      <c r="UG14" s="0"/>
-      <c r="UH14" s="0"/>
-      <c r="UI14" s="0"/>
-      <c r="UJ14" s="0"/>
-      <c r="UK14" s="0"/>
-      <c r="UL14" s="0"/>
-      <c r="UM14" s="0"/>
-      <c r="UN14" s="0"/>
-      <c r="UO14" s="0"/>
-      <c r="UP14" s="0"/>
-      <c r="UQ14" s="0"/>
-      <c r="UR14" s="0"/>
-      <c r="US14" s="0"/>
-      <c r="UT14" s="0"/>
-      <c r="UU14" s="0"/>
-      <c r="UV14" s="0"/>
-      <c r="UW14" s="0"/>
-      <c r="UX14" s="0"/>
-      <c r="UY14" s="0"/>
-      <c r="UZ14" s="0"/>
-      <c r="VA14" s="0"/>
-      <c r="VB14" s="0"/>
-      <c r="VC14" s="0"/>
-      <c r="VD14" s="0"/>
-      <c r="VE14" s="0"/>
-      <c r="VF14" s="0"/>
-      <c r="VG14" s="0"/>
-      <c r="VH14" s="0"/>
-      <c r="VI14" s="0"/>
-      <c r="VJ14" s="0"/>
-      <c r="VK14" s="0"/>
-      <c r="VL14" s="0"/>
-      <c r="VM14" s="0"/>
-      <c r="VN14" s="0"/>
-      <c r="VO14" s="0"/>
-      <c r="VP14" s="0"/>
-      <c r="VQ14" s="0"/>
-      <c r="VR14" s="0"/>
-      <c r="VS14" s="0"/>
-      <c r="VT14" s="0"/>
-      <c r="VU14" s="0"/>
-      <c r="VV14" s="0"/>
-      <c r="VW14" s="0"/>
-      <c r="VX14" s="0"/>
-      <c r="VY14" s="0"/>
-      <c r="VZ14" s="0"/>
-      <c r="WA14" s="0"/>
-      <c r="WB14" s="0"/>
-      <c r="WC14" s="0"/>
-      <c r="WD14" s="0"/>
-      <c r="WE14" s="0"/>
-      <c r="WF14" s="0"/>
-      <c r="WG14" s="0"/>
-      <c r="WH14" s="0"/>
-      <c r="WI14" s="0"/>
-      <c r="WJ14" s="0"/>
-      <c r="WK14" s="0"/>
-      <c r="WL14" s="0"/>
-      <c r="WM14" s="0"/>
-      <c r="WN14" s="0"/>
-      <c r="WO14" s="0"/>
-      <c r="WP14" s="0"/>
-      <c r="WQ14" s="0"/>
-      <c r="WR14" s="0"/>
-      <c r="WS14" s="0"/>
-      <c r="WT14" s="0"/>
-      <c r="WU14" s="0"/>
-      <c r="WV14" s="0"/>
-      <c r="WW14" s="0"/>
-      <c r="WX14" s="0"/>
-      <c r="WY14" s="0"/>
-      <c r="WZ14" s="0"/>
-      <c r="XA14" s="0"/>
-      <c r="XB14" s="0"/>
-      <c r="XC14" s="0"/>
-      <c r="XD14" s="0"/>
-      <c r="XE14" s="0"/>
-      <c r="XF14" s="0"/>
-      <c r="XG14" s="0"/>
-      <c r="XH14" s="0"/>
-      <c r="XI14" s="0"/>
-      <c r="XJ14" s="0"/>
-      <c r="XK14" s="0"/>
-      <c r="XL14" s="0"/>
-      <c r="XM14" s="0"/>
-      <c r="XN14" s="0"/>
-      <c r="XO14" s="0"/>
-      <c r="XP14" s="0"/>
-      <c r="XQ14" s="0"/>
-      <c r="XR14" s="0"/>
-      <c r="XS14" s="0"/>
-      <c r="XT14" s="0"/>
-      <c r="XU14" s="0"/>
-      <c r="XV14" s="0"/>
-      <c r="XW14" s="0"/>
-      <c r="XX14" s="0"/>
-      <c r="XY14" s="0"/>
-      <c r="XZ14" s="0"/>
-      <c r="YA14" s="0"/>
-      <c r="YB14" s="0"/>
-      <c r="YC14" s="0"/>
-      <c r="YD14" s="0"/>
-      <c r="YE14" s="0"/>
-      <c r="YF14" s="0"/>
-      <c r="YG14" s="0"/>
-      <c r="YH14" s="0"/>
-      <c r="YI14" s="0"/>
-      <c r="YJ14" s="0"/>
-      <c r="YK14" s="0"/>
-      <c r="YL14" s="0"/>
-      <c r="YM14" s="0"/>
-      <c r="YN14" s="0"/>
-      <c r="YO14" s="0"/>
-      <c r="YP14" s="0"/>
-      <c r="YQ14" s="0"/>
-      <c r="YR14" s="0"/>
-      <c r="YS14" s="0"/>
-      <c r="YT14" s="0"/>
-      <c r="YU14" s="0"/>
-      <c r="YV14" s="0"/>
-      <c r="YW14" s="0"/>
-      <c r="YX14" s="0"/>
-      <c r="YY14" s="0"/>
-      <c r="YZ14" s="0"/>
-      <c r="ZA14" s="0"/>
-      <c r="ZB14" s="0"/>
-      <c r="ZC14" s="0"/>
-      <c r="ZD14" s="0"/>
-      <c r="ZE14" s="0"/>
-      <c r="ZF14" s="0"/>
-      <c r="ZG14" s="0"/>
-      <c r="ZH14" s="0"/>
-      <c r="ZI14" s="0"/>
-      <c r="ZJ14" s="0"/>
-      <c r="ZK14" s="0"/>
-      <c r="ZL14" s="0"/>
-      <c r="ZM14" s="0"/>
-      <c r="ZN14" s="0"/>
-      <c r="ZO14" s="0"/>
-      <c r="ZP14" s="0"/>
-      <c r="ZQ14" s="0"/>
-      <c r="ZR14" s="0"/>
-      <c r="ZS14" s="0"/>
-      <c r="ZT14" s="0"/>
-      <c r="ZU14" s="0"/>
-      <c r="ZV14" s="0"/>
-      <c r="ZW14" s="0"/>
-      <c r="ZX14" s="0"/>
-      <c r="ZY14" s="0"/>
-      <c r="ZZ14" s="0"/>
-      <c r="AAA14" s="0"/>
-      <c r="AAB14" s="0"/>
-      <c r="AAC14" s="0"/>
-      <c r="AAD14" s="0"/>
-      <c r="AAE14" s="0"/>
-      <c r="AAF14" s="0"/>
-      <c r="AAG14" s="0"/>
-      <c r="AAH14" s="0"/>
-      <c r="AAI14" s="0"/>
-      <c r="AAJ14" s="0"/>
-      <c r="AAK14" s="0"/>
-      <c r="AAL14" s="0"/>
-      <c r="AAM14" s="0"/>
-      <c r="AAN14" s="0"/>
-      <c r="AAO14" s="0"/>
-      <c r="AAP14" s="0"/>
-      <c r="AAQ14" s="0"/>
-      <c r="AAR14" s="0"/>
-      <c r="AAS14" s="0"/>
-      <c r="AAT14" s="0"/>
-      <c r="AAU14" s="0"/>
-      <c r="AAV14" s="0"/>
-      <c r="AAW14" s="0"/>
-      <c r="AAX14" s="0"/>
-      <c r="AAY14" s="0"/>
-      <c r="AAZ14" s="0"/>
-      <c r="ABA14" s="0"/>
-      <c r="ABB14" s="0"/>
-      <c r="ABC14" s="0"/>
-      <c r="ABD14" s="0"/>
-      <c r="ABE14" s="0"/>
-      <c r="ABF14" s="0"/>
-      <c r="ABG14" s="0"/>
-      <c r="ABH14" s="0"/>
-      <c r="ABI14" s="0"/>
-      <c r="ABJ14" s="0"/>
-      <c r="ABK14" s="0"/>
-      <c r="ABL14" s="0"/>
-      <c r="ABM14" s="0"/>
-      <c r="ABN14" s="0"/>
-      <c r="ABO14" s="0"/>
-      <c r="ABP14" s="0"/>
-      <c r="ABQ14" s="0"/>
-      <c r="ABR14" s="0"/>
-      <c r="ABS14" s="0"/>
-      <c r="ABT14" s="0"/>
-      <c r="ABU14" s="0"/>
-      <c r="ABV14" s="0"/>
-      <c r="ABW14" s="0"/>
-      <c r="ABX14" s="0"/>
-      <c r="ABY14" s="0"/>
-      <c r="ABZ14" s="0"/>
-      <c r="ACA14" s="0"/>
-      <c r="ACB14" s="0"/>
-      <c r="ACC14" s="0"/>
-      <c r="ACD14" s="0"/>
-      <c r="ACE14" s="0"/>
-      <c r="ACF14" s="0"/>
-      <c r="ACG14" s="0"/>
-      <c r="ACH14" s="0"/>
-      <c r="ACI14" s="0"/>
-      <c r="ACJ14" s="0"/>
-      <c r="ACK14" s="0"/>
-      <c r="ACL14" s="0"/>
-      <c r="ACM14" s="0"/>
-      <c r="ACN14" s="0"/>
-      <c r="ACO14" s="0"/>
-      <c r="ACP14" s="0"/>
-      <c r="ACQ14" s="0"/>
-      <c r="ACR14" s="0"/>
-      <c r="ACS14" s="0"/>
-      <c r="ACT14" s="0"/>
-      <c r="ACU14" s="0"/>
-      <c r="ACV14" s="0"/>
-      <c r="ACW14" s="0"/>
-      <c r="ACX14" s="0"/>
-      <c r="ACY14" s="0"/>
-      <c r="ACZ14" s="0"/>
-      <c r="ADA14" s="0"/>
-      <c r="ADB14" s="0"/>
-      <c r="ADC14" s="0"/>
-      <c r="ADD14" s="0"/>
-      <c r="ADE14" s="0"/>
-      <c r="ADF14" s="0"/>
-      <c r="ADG14" s="0"/>
-      <c r="ADH14" s="0"/>
-      <c r="ADI14" s="0"/>
-      <c r="ADJ14" s="0"/>
-      <c r="ADK14" s="0"/>
-      <c r="ADL14" s="0"/>
-      <c r="ADM14" s="0"/>
-      <c r="ADN14" s="0"/>
-      <c r="ADO14" s="0"/>
-      <c r="ADP14" s="0"/>
-      <c r="ADQ14" s="0"/>
-      <c r="ADR14" s="0"/>
-      <c r="ADS14" s="0"/>
-      <c r="ADT14" s="0"/>
-      <c r="ADU14" s="0"/>
-      <c r="ADV14" s="0"/>
-      <c r="ADW14" s="0"/>
-      <c r="ADX14" s="0"/>
-      <c r="ADY14" s="0"/>
-      <c r="ADZ14" s="0"/>
-      <c r="AEA14" s="0"/>
-      <c r="AEB14" s="0"/>
-      <c r="AEC14" s="0"/>
-      <c r="AED14" s="0"/>
-      <c r="AEE14" s="0"/>
-      <c r="AEF14" s="0"/>
-      <c r="AEG14" s="0"/>
-      <c r="AEH14" s="0"/>
-      <c r="AEI14" s="0"/>
-      <c r="AEJ14" s="0"/>
-      <c r="AEK14" s="0"/>
-      <c r="AEL14" s="0"/>
-      <c r="AEM14" s="0"/>
-      <c r="AEN14" s="0"/>
-      <c r="AEO14" s="0"/>
-      <c r="AEP14" s="0"/>
-      <c r="AEQ14" s="0"/>
-      <c r="AER14" s="0"/>
-      <c r="AES14" s="0"/>
-      <c r="AET14" s="0"/>
-      <c r="AEU14" s="0"/>
-      <c r="AEV14" s="0"/>
-      <c r="AEW14" s="0"/>
-      <c r="AEX14" s="0"/>
-      <c r="AEY14" s="0"/>
-      <c r="AEZ14" s="0"/>
-      <c r="AFA14" s="0"/>
-      <c r="AFB14" s="0"/>
-      <c r="AFC14" s="0"/>
-      <c r="AFD14" s="0"/>
-      <c r="AFE14" s="0"/>
-      <c r="AFF14" s="0"/>
-      <c r="AFG14" s="0"/>
-      <c r="AFH14" s="0"/>
-      <c r="AFI14" s="0"/>
-      <c r="AFJ14" s="0"/>
-      <c r="AFK14" s="0"/>
-      <c r="AFL14" s="0"/>
-      <c r="AFM14" s="0"/>
-      <c r="AFN14" s="0"/>
-      <c r="AFO14" s="0"/>
-      <c r="AFP14" s="0"/>
-      <c r="AFQ14" s="0"/>
-      <c r="AFR14" s="0"/>
-      <c r="AFS14" s="0"/>
-      <c r="AFT14" s="0"/>
-      <c r="AFU14" s="0"/>
-      <c r="AFV14" s="0"/>
-      <c r="AFW14" s="0"/>
-      <c r="AFX14" s="0"/>
-      <c r="AFY14" s="0"/>
-      <c r="AFZ14" s="0"/>
-      <c r="AGA14" s="0"/>
-      <c r="AGB14" s="0"/>
-      <c r="AGC14" s="0"/>
-      <c r="AGD14" s="0"/>
-      <c r="AGE14" s="0"/>
-      <c r="AGF14" s="0"/>
-      <c r="AGG14" s="0"/>
-      <c r="AGH14" s="0"/>
-      <c r="AGI14" s="0"/>
-      <c r="AGJ14" s="0"/>
-      <c r="AGK14" s="0"/>
-      <c r="AGL14" s="0"/>
-      <c r="AGM14" s="0"/>
-      <c r="AGN14" s="0"/>
-      <c r="AGO14" s="0"/>
-      <c r="AGP14" s="0"/>
-      <c r="AGQ14" s="0"/>
-      <c r="AGR14" s="0"/>
-      <c r="AGS14" s="0"/>
-      <c r="AGT14" s="0"/>
-      <c r="AGU14" s="0"/>
-      <c r="AGV14" s="0"/>
-      <c r="AGW14" s="0"/>
-      <c r="AGX14" s="0"/>
-      <c r="AGY14" s="0"/>
-      <c r="AGZ14" s="0"/>
-      <c r="AHA14" s="0"/>
-      <c r="AHB14" s="0"/>
-      <c r="AHC14" s="0"/>
-      <c r="AHD14" s="0"/>
-      <c r="AHE14" s="0"/>
-      <c r="AHF14" s="0"/>
-      <c r="AHG14" s="0"/>
-      <c r="AHH14" s="0"/>
-      <c r="AHI14" s="0"/>
-      <c r="AHJ14" s="0"/>
-      <c r="AHK14" s="0"/>
-      <c r="AHL14" s="0"/>
-      <c r="AHM14" s="0"/>
-      <c r="AHN14" s="0"/>
-      <c r="AHO14" s="0"/>
-      <c r="AHP14" s="0"/>
-      <c r="AHQ14" s="0"/>
-      <c r="AHR14" s="0"/>
-      <c r="AHS14" s="0"/>
-      <c r="AHT14" s="0"/>
-      <c r="AHU14" s="0"/>
-      <c r="AHV14" s="0"/>
-      <c r="AHW14" s="0"/>
-      <c r="AHX14" s="0"/>
-      <c r="AHY14" s="0"/>
-      <c r="AHZ14" s="0"/>
-      <c r="AIA14" s="0"/>
-      <c r="AIB14" s="0"/>
-      <c r="AIC14" s="0"/>
-      <c r="AID14" s="0"/>
-      <c r="AIE14" s="0"/>
-      <c r="AIF14" s="0"/>
-      <c r="AIG14" s="0"/>
-      <c r="AIH14" s="0"/>
-      <c r="AII14" s="0"/>
-      <c r="AIJ14" s="0"/>
-      <c r="AIK14" s="0"/>
-      <c r="AIL14" s="0"/>
-      <c r="AIM14" s="0"/>
-      <c r="AIN14" s="0"/>
-      <c r="AIO14" s="0"/>
-      <c r="AIP14" s="0"/>
-      <c r="AIQ14" s="0"/>
-      <c r="AIR14" s="0"/>
-      <c r="AIS14" s="0"/>
-      <c r="AIT14" s="0"/>
-      <c r="AIU14" s="0"/>
-      <c r="AIV14" s="0"/>
-      <c r="AIW14" s="0"/>
-      <c r="AIX14" s="0"/>
-      <c r="AIY14" s="0"/>
-      <c r="AIZ14" s="0"/>
-      <c r="AJA14" s="0"/>
-      <c r="AJB14" s="0"/>
-      <c r="AJC14" s="0"/>
-      <c r="AJD14" s="0"/>
-      <c r="AJE14" s="0"/>
-      <c r="AJF14" s="0"/>
-      <c r="AJG14" s="0"/>
-      <c r="AJH14" s="0"/>
-      <c r="AJI14" s="0"/>
-      <c r="AJJ14" s="0"/>
-      <c r="AJK14" s="0"/>
-      <c r="AJL14" s="0"/>
-      <c r="AJM14" s="0"/>
-      <c r="AJN14" s="0"/>
-      <c r="AJO14" s="0"/>
-      <c r="AJP14" s="0"/>
-      <c r="AJQ14" s="0"/>
-      <c r="AJR14" s="0"/>
-      <c r="AJS14" s="0"/>
-      <c r="AJT14" s="0"/>
-      <c r="AJU14" s="0"/>
-      <c r="AJV14" s="0"/>
-      <c r="AJW14" s="0"/>
-      <c r="AJX14" s="0"/>
-      <c r="AJY14" s="0"/>
-      <c r="AJZ14" s="0"/>
-      <c r="AKA14" s="0"/>
-      <c r="AKB14" s="0"/>
-      <c r="AKC14" s="0"/>
-      <c r="AKD14" s="0"/>
-      <c r="AKE14" s="0"/>
-      <c r="AKF14" s="0"/>
-      <c r="AKG14" s="0"/>
-      <c r="AKH14" s="0"/>
-      <c r="AKI14" s="0"/>
-      <c r="AKJ14" s="0"/>
-      <c r="AKK14" s="0"/>
-      <c r="AKL14" s="0"/>
-      <c r="AKM14" s="0"/>
-      <c r="AKN14" s="0"/>
-      <c r="AKO14" s="0"/>
-      <c r="AKP14" s="0"/>
-      <c r="AKQ14" s="0"/>
-      <c r="AKR14" s="0"/>
-      <c r="AKS14" s="0"/>
-      <c r="AKT14" s="0"/>
-      <c r="AKU14" s="0"/>
-      <c r="AKV14" s="0"/>
-      <c r="AKW14" s="0"/>
-      <c r="AKX14" s="0"/>
-      <c r="AKY14" s="0"/>
-      <c r="AKZ14" s="0"/>
-      <c r="ALA14" s="0"/>
-      <c r="ALB14" s="0"/>
-      <c r="ALC14" s="0"/>
-      <c r="ALD14" s="0"/>
-      <c r="ALE14" s="0"/>
-      <c r="ALF14" s="0"/>
-      <c r="ALG14" s="0"/>
-      <c r="ALH14" s="0"/>
-      <c r="ALI14" s="0"/>
-      <c r="ALJ14" s="0"/>
-      <c r="ALK14" s="0"/>
-      <c r="ALL14" s="0"/>
-      <c r="ALM14" s="0"/>
-      <c r="ALN14" s="0"/>
-      <c r="ALO14" s="0"/>
-      <c r="ALP14" s="0"/>
-      <c r="ALQ14" s="0"/>
-      <c r="ALR14" s="0"/>
-      <c r="ALS14" s="0"/>
-      <c r="ALT14" s="0"/>
-      <c r="ALU14" s="0"/>
-      <c r="ALV14" s="0"/>
-      <c r="ALW14" s="0"/>
-      <c r="ALX14" s="0"/>
-      <c r="ALY14" s="0"/>
-      <c r="ALZ14" s="0"/>
-      <c r="AMA14" s="0"/>
-      <c r="AMB14" s="0"/>
-      <c r="AMC14" s="0"/>
-      <c r="AMD14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="15" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="15" t="e">
-        <f aca="true">INDIRECT( "G" &amp; ROW() )+INDIRECT( "F" &amp; ROW() )</f>
-        <v>#VALUE!</v>
+      <c r="G15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>23</v>
       </c>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
@@ -14925,14 +12877,23 @@
       <c r="AMD15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="22" t="e">
+        <f aca="true">INDIRECT( "G" &amp; ROW() )+INDIRECT( "F" &amp; ROW() )</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="I16" s="0"/>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
@@ -15945,19 +13906,17 @@
       <c r="AMD16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
       <c r="N17" s="0"/>
@@ -16966,20 +14925,20 @@
       <c r="AMC17" s="0"/>
       <c r="AMD17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
+    <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="2" t="s">
+        <v>33</v>
       </c>
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="27"/>
+      <c r="H18" s="0"/>
       <c r="I18" s="0"/>
-      <c r="J18" s="0"/>
-      <c r="K18" s="0"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
@@ -17989,20 +15948,16 @@
       <c r="AMD18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>32</v>
+      <c r="A19" s="1" t="s">
+        <v>34</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="0"/>
       <c r="C19" s="0"/>
       <c r="D19" s="0"/>
-      <c r="E19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="25"/>
       <c r="I19" s="0"/>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
@@ -19018,12 +16973,16 @@
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="0"/>
       <c r="D20" s="0"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
       <c r="J20" s="0"/>
@@ -20036,14 +17995,16 @@
       <c r="AMC20" s="0"/>
       <c r="AMD20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28"/>
-      <c r="B21" s="0"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="25"/>
       <c r="C21" s="0"/>
       <c r="D21" s="0"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
@@ -21057,13 +19018,13 @@
       <c r="AMD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
       <c r="D22" s="0"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
@@ -22077,13 +20038,13 @@
       <c r="AMD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
       <c r="D23" s="0"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
@@ -23097,13 +21058,13 @@
       <c r="AMD23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
@@ -24116,52 +22077,1072 @@
       <c r="AMC24" s="0"/>
       <c r="AMD24" s="0"/>
     </row>
-    <row r="25" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="26"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
       <c r="D25" s="0"/>
-      <c r="E25" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29" t="s">
-        <v>38</v>
-      </c>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
-      <c r="K25" s="31"/>
-      <c r="AME25" s="31"/>
-      <c r="AMF25" s="31"/>
-      <c r="AMG25" s="0"/>
-      <c r="AMH25" s="0"/>
-      <c r="AMI25" s="0"/>
-      <c r="AMJ25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="N25" s="0"/>
+      <c r="O25" s="0"/>
+      <c r="P25" s="0"/>
+      <c r="Q25" s="0"/>
+      <c r="R25" s="0"/>
+      <c r="S25" s="0"/>
+      <c r="T25" s="0"/>
+      <c r="U25" s="0"/>
+      <c r="V25" s="0"/>
+      <c r="W25" s="0"/>
+      <c r="X25" s="0"/>
+      <c r="Y25" s="0"/>
+      <c r="Z25" s="0"/>
+      <c r="AA25" s="0"/>
+      <c r="AB25" s="0"/>
+      <c r="AC25" s="0"/>
+      <c r="AD25" s="0"/>
+      <c r="AE25" s="0"/>
+      <c r="AF25" s="0"/>
+      <c r="AG25" s="0"/>
+      <c r="AH25" s="0"/>
+      <c r="AI25" s="0"/>
+      <c r="AJ25" s="0"/>
+      <c r="AK25" s="0"/>
+      <c r="AL25" s="0"/>
+      <c r="AM25" s="0"/>
+      <c r="AN25" s="0"/>
+      <c r="AO25" s="0"/>
+      <c r="AP25" s="0"/>
+      <c r="AQ25" s="0"/>
+      <c r="AR25" s="0"/>
+      <c r="AS25" s="0"/>
+      <c r="AT25" s="0"/>
+      <c r="AU25" s="0"/>
+      <c r="AV25" s="0"/>
+      <c r="AW25" s="0"/>
+      <c r="AX25" s="0"/>
+      <c r="AY25" s="0"/>
+      <c r="AZ25" s="0"/>
+      <c r="BA25" s="0"/>
+      <c r="BB25" s="0"/>
+      <c r="BC25" s="0"/>
+      <c r="BD25" s="0"/>
+      <c r="BE25" s="0"/>
+      <c r="BF25" s="0"/>
+      <c r="BG25" s="0"/>
+      <c r="BH25" s="0"/>
+      <c r="BI25" s="0"/>
+      <c r="BJ25" s="0"/>
+      <c r="BK25" s="0"/>
+      <c r="BL25" s="0"/>
+      <c r="BM25" s="0"/>
+      <c r="BN25" s="0"/>
+      <c r="BO25" s="0"/>
+      <c r="BP25" s="0"/>
+      <c r="BQ25" s="0"/>
+      <c r="BR25" s="0"/>
+      <c r="BS25" s="0"/>
+      <c r="BT25" s="0"/>
+      <c r="BU25" s="0"/>
+      <c r="BV25" s="0"/>
+      <c r="BW25" s="0"/>
+      <c r="BX25" s="0"/>
+      <c r="BY25" s="0"/>
+      <c r="BZ25" s="0"/>
+      <c r="CA25" s="0"/>
+      <c r="CB25" s="0"/>
+      <c r="CC25" s="0"/>
+      <c r="CD25" s="0"/>
+      <c r="CE25" s="0"/>
+      <c r="CF25" s="0"/>
+      <c r="CG25" s="0"/>
+      <c r="CH25" s="0"/>
+      <c r="CI25" s="0"/>
+      <c r="CJ25" s="0"/>
+      <c r="CK25" s="0"/>
+      <c r="CL25" s="0"/>
+      <c r="CM25" s="0"/>
+      <c r="CN25" s="0"/>
+      <c r="CO25" s="0"/>
+      <c r="CP25" s="0"/>
+      <c r="CQ25" s="0"/>
+      <c r="CR25" s="0"/>
+      <c r="CS25" s="0"/>
+      <c r="CT25" s="0"/>
+      <c r="CU25" s="0"/>
+      <c r="CV25" s="0"/>
+      <c r="CW25" s="0"/>
+      <c r="CX25" s="0"/>
+      <c r="CY25" s="0"/>
+      <c r="CZ25" s="0"/>
+      <c r="DA25" s="0"/>
+      <c r="DB25" s="0"/>
+      <c r="DC25" s="0"/>
+      <c r="DD25" s="0"/>
+      <c r="DE25" s="0"/>
+      <c r="DF25" s="0"/>
+      <c r="DG25" s="0"/>
+      <c r="DH25" s="0"/>
+      <c r="DI25" s="0"/>
+      <c r="DJ25" s="0"/>
+      <c r="DK25" s="0"/>
+      <c r="DL25" s="0"/>
+      <c r="DM25" s="0"/>
+      <c r="DN25" s="0"/>
+      <c r="DO25" s="0"/>
+      <c r="DP25" s="0"/>
+      <c r="DQ25" s="0"/>
+      <c r="DR25" s="0"/>
+      <c r="DS25" s="0"/>
+      <c r="DT25" s="0"/>
+      <c r="DU25" s="0"/>
+      <c r="DV25" s="0"/>
+      <c r="DW25" s="0"/>
+      <c r="DX25" s="0"/>
+      <c r="DY25" s="0"/>
+      <c r="DZ25" s="0"/>
+      <c r="EA25" s="0"/>
+      <c r="EB25" s="0"/>
+      <c r="EC25" s="0"/>
+      <c r="ED25" s="0"/>
+      <c r="EE25" s="0"/>
+      <c r="EF25" s="0"/>
+      <c r="EG25" s="0"/>
+      <c r="EH25" s="0"/>
+      <c r="EI25" s="0"/>
+      <c r="EJ25" s="0"/>
+      <c r="EK25" s="0"/>
+      <c r="EL25" s="0"/>
+      <c r="EM25" s="0"/>
+      <c r="EN25" s="0"/>
+      <c r="EO25" s="0"/>
+      <c r="EP25" s="0"/>
+      <c r="EQ25" s="0"/>
+      <c r="ER25" s="0"/>
+      <c r="ES25" s="0"/>
+      <c r="ET25" s="0"/>
+      <c r="EU25" s="0"/>
+      <c r="EV25" s="0"/>
+      <c r="EW25" s="0"/>
+      <c r="EX25" s="0"/>
+      <c r="EY25" s="0"/>
+      <c r="EZ25" s="0"/>
+      <c r="FA25" s="0"/>
+      <c r="FB25" s="0"/>
+      <c r="FC25" s="0"/>
+      <c r="FD25" s="0"/>
+      <c r="FE25" s="0"/>
+      <c r="FF25" s="0"/>
+      <c r="FG25" s="0"/>
+      <c r="FH25" s="0"/>
+      <c r="FI25" s="0"/>
+      <c r="FJ25" s="0"/>
+      <c r="FK25" s="0"/>
+      <c r="FL25" s="0"/>
+      <c r="FM25" s="0"/>
+      <c r="FN25" s="0"/>
+      <c r="FO25" s="0"/>
+      <c r="FP25" s="0"/>
+      <c r="FQ25" s="0"/>
+      <c r="FR25" s="0"/>
+      <c r="FS25" s="0"/>
+      <c r="FT25" s="0"/>
+      <c r="FU25" s="0"/>
+      <c r="FV25" s="0"/>
+      <c r="FW25" s="0"/>
+      <c r="FX25" s="0"/>
+      <c r="FY25" s="0"/>
+      <c r="FZ25" s="0"/>
+      <c r="GA25" s="0"/>
+      <c r="GB25" s="0"/>
+      <c r="GC25" s="0"/>
+      <c r="GD25" s="0"/>
+      <c r="GE25" s="0"/>
+      <c r="GF25" s="0"/>
+      <c r="GG25" s="0"/>
+      <c r="GH25" s="0"/>
+      <c r="GI25" s="0"/>
+      <c r="GJ25" s="0"/>
+      <c r="GK25" s="0"/>
+      <c r="GL25" s="0"/>
+      <c r="GM25" s="0"/>
+      <c r="GN25" s="0"/>
+      <c r="GO25" s="0"/>
+      <c r="GP25" s="0"/>
+      <c r="GQ25" s="0"/>
+      <c r="GR25" s="0"/>
+      <c r="GS25" s="0"/>
+      <c r="GT25" s="0"/>
+      <c r="GU25" s="0"/>
+      <c r="GV25" s="0"/>
+      <c r="GW25" s="0"/>
+      <c r="GX25" s="0"/>
+      <c r="GY25" s="0"/>
+      <c r="GZ25" s="0"/>
+      <c r="HA25" s="0"/>
+      <c r="HB25" s="0"/>
+      <c r="HC25" s="0"/>
+      <c r="HD25" s="0"/>
+      <c r="HE25" s="0"/>
+      <c r="HF25" s="0"/>
+      <c r="HG25" s="0"/>
+      <c r="HH25" s="0"/>
+      <c r="HI25" s="0"/>
+      <c r="HJ25" s="0"/>
+      <c r="HK25" s="0"/>
+      <c r="HL25" s="0"/>
+      <c r="HM25" s="0"/>
+      <c r="HN25" s="0"/>
+      <c r="HO25" s="0"/>
+      <c r="HP25" s="0"/>
+      <c r="HQ25" s="0"/>
+      <c r="HR25" s="0"/>
+      <c r="HS25" s="0"/>
+      <c r="HT25" s="0"/>
+      <c r="HU25" s="0"/>
+      <c r="HV25" s="0"/>
+      <c r="HW25" s="0"/>
+      <c r="HX25" s="0"/>
+      <c r="HY25" s="0"/>
+      <c r="HZ25" s="0"/>
+      <c r="IA25" s="0"/>
+      <c r="IB25" s="0"/>
+      <c r="IC25" s="0"/>
+      <c r="ID25" s="0"/>
+      <c r="IE25" s="0"/>
+      <c r="IF25" s="0"/>
+      <c r="IG25" s="0"/>
+      <c r="IH25" s="0"/>
+      <c r="II25" s="0"/>
+      <c r="IJ25" s="0"/>
+      <c r="IK25" s="0"/>
+      <c r="IL25" s="0"/>
+      <c r="IM25" s="0"/>
+      <c r="IN25" s="0"/>
+      <c r="IO25" s="0"/>
+      <c r="IP25" s="0"/>
+      <c r="IQ25" s="0"/>
+      <c r="IR25" s="0"/>
+      <c r="IS25" s="0"/>
+      <c r="IT25" s="0"/>
+      <c r="IU25" s="0"/>
+      <c r="IV25" s="0"/>
+      <c r="IW25" s="0"/>
+      <c r="IX25" s="0"/>
+      <c r="IY25" s="0"/>
+      <c r="IZ25" s="0"/>
+      <c r="JA25" s="0"/>
+      <c r="JB25" s="0"/>
+      <c r="JC25" s="0"/>
+      <c r="JD25" s="0"/>
+      <c r="JE25" s="0"/>
+      <c r="JF25" s="0"/>
+      <c r="JG25" s="0"/>
+      <c r="JH25" s="0"/>
+      <c r="JI25" s="0"/>
+      <c r="JJ25" s="0"/>
+      <c r="JK25" s="0"/>
+      <c r="JL25" s="0"/>
+      <c r="JM25" s="0"/>
+      <c r="JN25" s="0"/>
+      <c r="JO25" s="0"/>
+      <c r="JP25" s="0"/>
+      <c r="JQ25" s="0"/>
+      <c r="JR25" s="0"/>
+      <c r="JS25" s="0"/>
+      <c r="JT25" s="0"/>
+      <c r="JU25" s="0"/>
+      <c r="JV25" s="0"/>
+      <c r="JW25" s="0"/>
+      <c r="JX25" s="0"/>
+      <c r="JY25" s="0"/>
+      <c r="JZ25" s="0"/>
+      <c r="KA25" s="0"/>
+      <c r="KB25" s="0"/>
+      <c r="KC25" s="0"/>
+      <c r="KD25" s="0"/>
+      <c r="KE25" s="0"/>
+      <c r="KF25" s="0"/>
+      <c r="KG25" s="0"/>
+      <c r="KH25" s="0"/>
+      <c r="KI25" s="0"/>
+      <c r="KJ25" s="0"/>
+      <c r="KK25" s="0"/>
+      <c r="KL25" s="0"/>
+      <c r="KM25" s="0"/>
+      <c r="KN25" s="0"/>
+      <c r="KO25" s="0"/>
+      <c r="KP25" s="0"/>
+      <c r="KQ25" s="0"/>
+      <c r="KR25" s="0"/>
+      <c r="KS25" s="0"/>
+      <c r="KT25" s="0"/>
+      <c r="KU25" s="0"/>
+      <c r="KV25" s="0"/>
+      <c r="KW25" s="0"/>
+      <c r="KX25" s="0"/>
+      <c r="KY25" s="0"/>
+      <c r="KZ25" s="0"/>
+      <c r="LA25" s="0"/>
+      <c r="LB25" s="0"/>
+      <c r="LC25" s="0"/>
+      <c r="LD25" s="0"/>
+      <c r="LE25" s="0"/>
+      <c r="LF25" s="0"/>
+      <c r="LG25" s="0"/>
+      <c r="LH25" s="0"/>
+      <c r="LI25" s="0"/>
+      <c r="LJ25" s="0"/>
+      <c r="LK25" s="0"/>
+      <c r="LL25" s="0"/>
+      <c r="LM25" s="0"/>
+      <c r="LN25" s="0"/>
+      <c r="LO25" s="0"/>
+      <c r="LP25" s="0"/>
+      <c r="LQ25" s="0"/>
+      <c r="LR25" s="0"/>
+      <c r="LS25" s="0"/>
+      <c r="LT25" s="0"/>
+      <c r="LU25" s="0"/>
+      <c r="LV25" s="0"/>
+      <c r="LW25" s="0"/>
+      <c r="LX25" s="0"/>
+      <c r="LY25" s="0"/>
+      <c r="LZ25" s="0"/>
+      <c r="MA25" s="0"/>
+      <c r="MB25" s="0"/>
+      <c r="MC25" s="0"/>
+      <c r="MD25" s="0"/>
+      <c r="ME25" s="0"/>
+      <c r="MF25" s="0"/>
+      <c r="MG25" s="0"/>
+      <c r="MH25" s="0"/>
+      <c r="MI25" s="0"/>
+      <c r="MJ25" s="0"/>
+      <c r="MK25" s="0"/>
+      <c r="ML25" s="0"/>
+      <c r="MM25" s="0"/>
+      <c r="MN25" s="0"/>
+      <c r="MO25" s="0"/>
+      <c r="MP25" s="0"/>
+      <c r="MQ25" s="0"/>
+      <c r="MR25" s="0"/>
+      <c r="MS25" s="0"/>
+      <c r="MT25" s="0"/>
+      <c r="MU25" s="0"/>
+      <c r="MV25" s="0"/>
+      <c r="MW25" s="0"/>
+      <c r="MX25" s="0"/>
+      <c r="MY25" s="0"/>
+      <c r="MZ25" s="0"/>
+      <c r="NA25" s="0"/>
+      <c r="NB25" s="0"/>
+      <c r="NC25" s="0"/>
+      <c r="ND25" s="0"/>
+      <c r="NE25" s="0"/>
+      <c r="NF25" s="0"/>
+      <c r="NG25" s="0"/>
+      <c r="NH25" s="0"/>
+      <c r="NI25" s="0"/>
+      <c r="NJ25" s="0"/>
+      <c r="NK25" s="0"/>
+      <c r="NL25" s="0"/>
+      <c r="NM25" s="0"/>
+      <c r="NN25" s="0"/>
+      <c r="NO25" s="0"/>
+      <c r="NP25" s="0"/>
+      <c r="NQ25" s="0"/>
+      <c r="NR25" s="0"/>
+      <c r="NS25" s="0"/>
+      <c r="NT25" s="0"/>
+      <c r="NU25" s="0"/>
+      <c r="NV25" s="0"/>
+      <c r="NW25" s="0"/>
+      <c r="NX25" s="0"/>
+      <c r="NY25" s="0"/>
+      <c r="NZ25" s="0"/>
+      <c r="OA25" s="0"/>
+      <c r="OB25" s="0"/>
+      <c r="OC25" s="0"/>
+      <c r="OD25" s="0"/>
+      <c r="OE25" s="0"/>
+      <c r="OF25" s="0"/>
+      <c r="OG25" s="0"/>
+      <c r="OH25" s="0"/>
+      <c r="OI25" s="0"/>
+      <c r="OJ25" s="0"/>
+      <c r="OK25" s="0"/>
+      <c r="OL25" s="0"/>
+      <c r="OM25" s="0"/>
+      <c r="ON25" s="0"/>
+      <c r="OO25" s="0"/>
+      <c r="OP25" s="0"/>
+      <c r="OQ25" s="0"/>
+      <c r="OR25" s="0"/>
+      <c r="OS25" s="0"/>
+      <c r="OT25" s="0"/>
+      <c r="OU25" s="0"/>
+      <c r="OV25" s="0"/>
+      <c r="OW25" s="0"/>
+      <c r="OX25" s="0"/>
+      <c r="OY25" s="0"/>
+      <c r="OZ25" s="0"/>
+      <c r="PA25" s="0"/>
+      <c r="PB25" s="0"/>
+      <c r="PC25" s="0"/>
+      <c r="PD25" s="0"/>
+      <c r="PE25" s="0"/>
+      <c r="PF25" s="0"/>
+      <c r="PG25" s="0"/>
+      <c r="PH25" s="0"/>
+      <c r="PI25" s="0"/>
+      <c r="PJ25" s="0"/>
+      <c r="PK25" s="0"/>
+      <c r="PL25" s="0"/>
+      <c r="PM25" s="0"/>
+      <c r="PN25" s="0"/>
+      <c r="PO25" s="0"/>
+      <c r="PP25" s="0"/>
+      <c r="PQ25" s="0"/>
+      <c r="PR25" s="0"/>
+      <c r="PS25" s="0"/>
+      <c r="PT25" s="0"/>
+      <c r="PU25" s="0"/>
+      <c r="PV25" s="0"/>
+      <c r="PW25" s="0"/>
+      <c r="PX25" s="0"/>
+      <c r="PY25" s="0"/>
+      <c r="PZ25" s="0"/>
+      <c r="QA25" s="0"/>
+      <c r="QB25" s="0"/>
+      <c r="QC25" s="0"/>
+      <c r="QD25" s="0"/>
+      <c r="QE25" s="0"/>
+      <c r="QF25" s="0"/>
+      <c r="QG25" s="0"/>
+      <c r="QH25" s="0"/>
+      <c r="QI25" s="0"/>
+      <c r="QJ25" s="0"/>
+      <c r="QK25" s="0"/>
+      <c r="QL25" s="0"/>
+      <c r="QM25" s="0"/>
+      <c r="QN25" s="0"/>
+      <c r="QO25" s="0"/>
+      <c r="QP25" s="0"/>
+      <c r="QQ25" s="0"/>
+      <c r="QR25" s="0"/>
+      <c r="QS25" s="0"/>
+      <c r="QT25" s="0"/>
+      <c r="QU25" s="0"/>
+      <c r="QV25" s="0"/>
+      <c r="QW25" s="0"/>
+      <c r="QX25" s="0"/>
+      <c r="QY25" s="0"/>
+      <c r="QZ25" s="0"/>
+      <c r="RA25" s="0"/>
+      <c r="RB25" s="0"/>
+      <c r="RC25" s="0"/>
+      <c r="RD25" s="0"/>
+      <c r="RE25" s="0"/>
+      <c r="RF25" s="0"/>
+      <c r="RG25" s="0"/>
+      <c r="RH25" s="0"/>
+      <c r="RI25" s="0"/>
+      <c r="RJ25" s="0"/>
+      <c r="RK25" s="0"/>
+      <c r="RL25" s="0"/>
+      <c r="RM25" s="0"/>
+      <c r="RN25" s="0"/>
+      <c r="RO25" s="0"/>
+      <c r="RP25" s="0"/>
+      <c r="RQ25" s="0"/>
+      <c r="RR25" s="0"/>
+      <c r="RS25" s="0"/>
+      <c r="RT25" s="0"/>
+      <c r="RU25" s="0"/>
+      <c r="RV25" s="0"/>
+      <c r="RW25" s="0"/>
+      <c r="RX25" s="0"/>
+      <c r="RY25" s="0"/>
+      <c r="RZ25" s="0"/>
+      <c r="SA25" s="0"/>
+      <c r="SB25" s="0"/>
+      <c r="SC25" s="0"/>
+      <c r="SD25" s="0"/>
+      <c r="SE25" s="0"/>
+      <c r="SF25" s="0"/>
+      <c r="SG25" s="0"/>
+      <c r="SH25" s="0"/>
+      <c r="SI25" s="0"/>
+      <c r="SJ25" s="0"/>
+      <c r="SK25" s="0"/>
+      <c r="SL25" s="0"/>
+      <c r="SM25" s="0"/>
+      <c r="SN25" s="0"/>
+      <c r="SO25" s="0"/>
+      <c r="SP25" s="0"/>
+      <c r="SQ25" s="0"/>
+      <c r="SR25" s="0"/>
+      <c r="SS25" s="0"/>
+      <c r="ST25" s="0"/>
+      <c r="SU25" s="0"/>
+      <c r="SV25" s="0"/>
+      <c r="SW25" s="0"/>
+      <c r="SX25" s="0"/>
+      <c r="SY25" s="0"/>
+      <c r="SZ25" s="0"/>
+      <c r="TA25" s="0"/>
+      <c r="TB25" s="0"/>
+      <c r="TC25" s="0"/>
+      <c r="TD25" s="0"/>
+      <c r="TE25" s="0"/>
+      <c r="TF25" s="0"/>
+      <c r="TG25" s="0"/>
+      <c r="TH25" s="0"/>
+      <c r="TI25" s="0"/>
+      <c r="TJ25" s="0"/>
+      <c r="TK25" s="0"/>
+      <c r="TL25" s="0"/>
+      <c r="TM25" s="0"/>
+      <c r="TN25" s="0"/>
+      <c r="TO25" s="0"/>
+      <c r="TP25" s="0"/>
+      <c r="TQ25" s="0"/>
+      <c r="TR25" s="0"/>
+      <c r="TS25" s="0"/>
+      <c r="TT25" s="0"/>
+      <c r="TU25" s="0"/>
+      <c r="TV25" s="0"/>
+      <c r="TW25" s="0"/>
+      <c r="TX25" s="0"/>
+      <c r="TY25" s="0"/>
+      <c r="TZ25" s="0"/>
+      <c r="UA25" s="0"/>
+      <c r="UB25" s="0"/>
+      <c r="UC25" s="0"/>
+      <c r="UD25" s="0"/>
+      <c r="UE25" s="0"/>
+      <c r="UF25" s="0"/>
+      <c r="UG25" s="0"/>
+      <c r="UH25" s="0"/>
+      <c r="UI25" s="0"/>
+      <c r="UJ25" s="0"/>
+      <c r="UK25" s="0"/>
+      <c r="UL25" s="0"/>
+      <c r="UM25" s="0"/>
+      <c r="UN25" s="0"/>
+      <c r="UO25" s="0"/>
+      <c r="UP25" s="0"/>
+      <c r="UQ25" s="0"/>
+      <c r="UR25" s="0"/>
+      <c r="US25" s="0"/>
+      <c r="UT25" s="0"/>
+      <c r="UU25" s="0"/>
+      <c r="UV25" s="0"/>
+      <c r="UW25" s="0"/>
+      <c r="UX25" s="0"/>
+      <c r="UY25" s="0"/>
+      <c r="UZ25" s="0"/>
+      <c r="VA25" s="0"/>
+      <c r="VB25" s="0"/>
+      <c r="VC25" s="0"/>
+      <c r="VD25" s="0"/>
+      <c r="VE25" s="0"/>
+      <c r="VF25" s="0"/>
+      <c r="VG25" s="0"/>
+      <c r="VH25" s="0"/>
+      <c r="VI25" s="0"/>
+      <c r="VJ25" s="0"/>
+      <c r="VK25" s="0"/>
+      <c r="VL25" s="0"/>
+      <c r="VM25" s="0"/>
+      <c r="VN25" s="0"/>
+      <c r="VO25" s="0"/>
+      <c r="VP25" s="0"/>
+      <c r="VQ25" s="0"/>
+      <c r="VR25" s="0"/>
+      <c r="VS25" s="0"/>
+      <c r="VT25" s="0"/>
+      <c r="VU25" s="0"/>
+      <c r="VV25" s="0"/>
+      <c r="VW25" s="0"/>
+      <c r="VX25" s="0"/>
+      <c r="VY25" s="0"/>
+      <c r="VZ25" s="0"/>
+      <c r="WA25" s="0"/>
+      <c r="WB25" s="0"/>
+      <c r="WC25" s="0"/>
+      <c r="WD25" s="0"/>
+      <c r="WE25" s="0"/>
+      <c r="WF25" s="0"/>
+      <c r="WG25" s="0"/>
+      <c r="WH25" s="0"/>
+      <c r="WI25" s="0"/>
+      <c r="WJ25" s="0"/>
+      <c r="WK25" s="0"/>
+      <c r="WL25" s="0"/>
+      <c r="WM25" s="0"/>
+      <c r="WN25" s="0"/>
+      <c r="WO25" s="0"/>
+      <c r="WP25" s="0"/>
+      <c r="WQ25" s="0"/>
+      <c r="WR25" s="0"/>
+      <c r="WS25" s="0"/>
+      <c r="WT25" s="0"/>
+      <c r="WU25" s="0"/>
+      <c r="WV25" s="0"/>
+      <c r="WW25" s="0"/>
+      <c r="WX25" s="0"/>
+      <c r="WY25" s="0"/>
+      <c r="WZ25" s="0"/>
+      <c r="XA25" s="0"/>
+      <c r="XB25" s="0"/>
+      <c r="XC25" s="0"/>
+      <c r="XD25" s="0"/>
+      <c r="XE25" s="0"/>
+      <c r="XF25" s="0"/>
+      <c r="XG25" s="0"/>
+      <c r="XH25" s="0"/>
+      <c r="XI25" s="0"/>
+      <c r="XJ25" s="0"/>
+      <c r="XK25" s="0"/>
+      <c r="XL25" s="0"/>
+      <c r="XM25" s="0"/>
+      <c r="XN25" s="0"/>
+      <c r="XO25" s="0"/>
+      <c r="XP25" s="0"/>
+      <c r="XQ25" s="0"/>
+      <c r="XR25" s="0"/>
+      <c r="XS25" s="0"/>
+      <c r="XT25" s="0"/>
+      <c r="XU25" s="0"/>
+      <c r="XV25" s="0"/>
+      <c r="XW25" s="0"/>
+      <c r="XX25" s="0"/>
+      <c r="XY25" s="0"/>
+      <c r="XZ25" s="0"/>
+      <c r="YA25" s="0"/>
+      <c r="YB25" s="0"/>
+      <c r="YC25" s="0"/>
+      <c r="YD25" s="0"/>
+      <c r="YE25" s="0"/>
+      <c r="YF25" s="0"/>
+      <c r="YG25" s="0"/>
+      <c r="YH25" s="0"/>
+      <c r="YI25" s="0"/>
+      <c r="YJ25" s="0"/>
+      <c r="YK25" s="0"/>
+      <c r="YL25" s="0"/>
+      <c r="YM25" s="0"/>
+      <c r="YN25" s="0"/>
+      <c r="YO25" s="0"/>
+      <c r="YP25" s="0"/>
+      <c r="YQ25" s="0"/>
+      <c r="YR25" s="0"/>
+      <c r="YS25" s="0"/>
+      <c r="YT25" s="0"/>
+      <c r="YU25" s="0"/>
+      <c r="YV25" s="0"/>
+      <c r="YW25" s="0"/>
+      <c r="YX25" s="0"/>
+      <c r="YY25" s="0"/>
+      <c r="YZ25" s="0"/>
+      <c r="ZA25" s="0"/>
+      <c r="ZB25" s="0"/>
+      <c r="ZC25" s="0"/>
+      <c r="ZD25" s="0"/>
+      <c r="ZE25" s="0"/>
+      <c r="ZF25" s="0"/>
+      <c r="ZG25" s="0"/>
+      <c r="ZH25" s="0"/>
+      <c r="ZI25" s="0"/>
+      <c r="ZJ25" s="0"/>
+      <c r="ZK25" s="0"/>
+      <c r="ZL25" s="0"/>
+      <c r="ZM25" s="0"/>
+      <c r="ZN25" s="0"/>
+      <c r="ZO25" s="0"/>
+      <c r="ZP25" s="0"/>
+      <c r="ZQ25" s="0"/>
+      <c r="ZR25" s="0"/>
+      <c r="ZS25" s="0"/>
+      <c r="ZT25" s="0"/>
+      <c r="ZU25" s="0"/>
+      <c r="ZV25" s="0"/>
+      <c r="ZW25" s="0"/>
+      <c r="ZX25" s="0"/>
+      <c r="ZY25" s="0"/>
+      <c r="ZZ25" s="0"/>
+      <c r="AAA25" s="0"/>
+      <c r="AAB25" s="0"/>
+      <c r="AAC25" s="0"/>
+      <c r="AAD25" s="0"/>
+      <c r="AAE25" s="0"/>
+      <c r="AAF25" s="0"/>
+      <c r="AAG25" s="0"/>
+      <c r="AAH25" s="0"/>
+      <c r="AAI25" s="0"/>
+      <c r="AAJ25" s="0"/>
+      <c r="AAK25" s="0"/>
+      <c r="AAL25" s="0"/>
+      <c r="AAM25" s="0"/>
+      <c r="AAN25" s="0"/>
+      <c r="AAO25" s="0"/>
+      <c r="AAP25" s="0"/>
+      <c r="AAQ25" s="0"/>
+      <c r="AAR25" s="0"/>
+      <c r="AAS25" s="0"/>
+      <c r="AAT25" s="0"/>
+      <c r="AAU25" s="0"/>
+      <c r="AAV25" s="0"/>
+      <c r="AAW25" s="0"/>
+      <c r="AAX25" s="0"/>
+      <c r="AAY25" s="0"/>
+      <c r="AAZ25" s="0"/>
+      <c r="ABA25" s="0"/>
+      <c r="ABB25" s="0"/>
+      <c r="ABC25" s="0"/>
+      <c r="ABD25" s="0"/>
+      <c r="ABE25" s="0"/>
+      <c r="ABF25" s="0"/>
+      <c r="ABG25" s="0"/>
+      <c r="ABH25" s="0"/>
+      <c r="ABI25" s="0"/>
+      <c r="ABJ25" s="0"/>
+      <c r="ABK25" s="0"/>
+      <c r="ABL25" s="0"/>
+      <c r="ABM25" s="0"/>
+      <c r="ABN25" s="0"/>
+      <c r="ABO25" s="0"/>
+      <c r="ABP25" s="0"/>
+      <c r="ABQ25" s="0"/>
+      <c r="ABR25" s="0"/>
+      <c r="ABS25" s="0"/>
+      <c r="ABT25" s="0"/>
+      <c r="ABU25" s="0"/>
+      <c r="ABV25" s="0"/>
+      <c r="ABW25" s="0"/>
+      <c r="ABX25" s="0"/>
+      <c r="ABY25" s="0"/>
+      <c r="ABZ25" s="0"/>
+      <c r="ACA25" s="0"/>
+      <c r="ACB25" s="0"/>
+      <c r="ACC25" s="0"/>
+      <c r="ACD25" s="0"/>
+      <c r="ACE25" s="0"/>
+      <c r="ACF25" s="0"/>
+      <c r="ACG25" s="0"/>
+      <c r="ACH25" s="0"/>
+      <c r="ACI25" s="0"/>
+      <c r="ACJ25" s="0"/>
+      <c r="ACK25" s="0"/>
+      <c r="ACL25" s="0"/>
+      <c r="ACM25" s="0"/>
+      <c r="ACN25" s="0"/>
+      <c r="ACO25" s="0"/>
+      <c r="ACP25" s="0"/>
+      <c r="ACQ25" s="0"/>
+      <c r="ACR25" s="0"/>
+      <c r="ACS25" s="0"/>
+      <c r="ACT25" s="0"/>
+      <c r="ACU25" s="0"/>
+      <c r="ACV25" s="0"/>
+      <c r="ACW25" s="0"/>
+      <c r="ACX25" s="0"/>
+      <c r="ACY25" s="0"/>
+      <c r="ACZ25" s="0"/>
+      <c r="ADA25" s="0"/>
+      <c r="ADB25" s="0"/>
+      <c r="ADC25" s="0"/>
+      <c r="ADD25" s="0"/>
+      <c r="ADE25" s="0"/>
+      <c r="ADF25" s="0"/>
+      <c r="ADG25" s="0"/>
+      <c r="ADH25" s="0"/>
+      <c r="ADI25" s="0"/>
+      <c r="ADJ25" s="0"/>
+      <c r="ADK25" s="0"/>
+      <c r="ADL25" s="0"/>
+      <c r="ADM25" s="0"/>
+      <c r="ADN25" s="0"/>
+      <c r="ADO25" s="0"/>
+      <c r="ADP25" s="0"/>
+      <c r="ADQ25" s="0"/>
+      <c r="ADR25" s="0"/>
+      <c r="ADS25" s="0"/>
+      <c r="ADT25" s="0"/>
+      <c r="ADU25" s="0"/>
+      <c r="ADV25" s="0"/>
+      <c r="ADW25" s="0"/>
+      <c r="ADX25" s="0"/>
+      <c r="ADY25" s="0"/>
+      <c r="ADZ25" s="0"/>
+      <c r="AEA25" s="0"/>
+      <c r="AEB25" s="0"/>
+      <c r="AEC25" s="0"/>
+      <c r="AED25" s="0"/>
+      <c r="AEE25" s="0"/>
+      <c r="AEF25" s="0"/>
+      <c r="AEG25" s="0"/>
+      <c r="AEH25" s="0"/>
+      <c r="AEI25" s="0"/>
+      <c r="AEJ25" s="0"/>
+      <c r="AEK25" s="0"/>
+      <c r="AEL25" s="0"/>
+      <c r="AEM25" s="0"/>
+      <c r="AEN25" s="0"/>
+      <c r="AEO25" s="0"/>
+      <c r="AEP25" s="0"/>
+      <c r="AEQ25" s="0"/>
+      <c r="AER25" s="0"/>
+      <c r="AES25" s="0"/>
+      <c r="AET25" s="0"/>
+      <c r="AEU25" s="0"/>
+      <c r="AEV25" s="0"/>
+      <c r="AEW25" s="0"/>
+      <c r="AEX25" s="0"/>
+      <c r="AEY25" s="0"/>
+      <c r="AEZ25" s="0"/>
+      <c r="AFA25" s="0"/>
+      <c r="AFB25" s="0"/>
+      <c r="AFC25" s="0"/>
+      <c r="AFD25" s="0"/>
+      <c r="AFE25" s="0"/>
+      <c r="AFF25" s="0"/>
+      <c r="AFG25" s="0"/>
+      <c r="AFH25" s="0"/>
+      <c r="AFI25" s="0"/>
+      <c r="AFJ25" s="0"/>
+      <c r="AFK25" s="0"/>
+      <c r="AFL25" s="0"/>
+      <c r="AFM25" s="0"/>
+      <c r="AFN25" s="0"/>
+      <c r="AFO25" s="0"/>
+      <c r="AFP25" s="0"/>
+      <c r="AFQ25" s="0"/>
+      <c r="AFR25" s="0"/>
+      <c r="AFS25" s="0"/>
+      <c r="AFT25" s="0"/>
+      <c r="AFU25" s="0"/>
+      <c r="AFV25" s="0"/>
+      <c r="AFW25" s="0"/>
+      <c r="AFX25" s="0"/>
+      <c r="AFY25" s="0"/>
+      <c r="AFZ25" s="0"/>
+      <c r="AGA25" s="0"/>
+      <c r="AGB25" s="0"/>
+      <c r="AGC25" s="0"/>
+      <c r="AGD25" s="0"/>
+      <c r="AGE25" s="0"/>
+      <c r="AGF25" s="0"/>
+      <c r="AGG25" s="0"/>
+      <c r="AGH25" s="0"/>
+      <c r="AGI25" s="0"/>
+      <c r="AGJ25" s="0"/>
+      <c r="AGK25" s="0"/>
+      <c r="AGL25" s="0"/>
+      <c r="AGM25" s="0"/>
+      <c r="AGN25" s="0"/>
+      <c r="AGO25" s="0"/>
+      <c r="AGP25" s="0"/>
+      <c r="AGQ25" s="0"/>
+      <c r="AGR25" s="0"/>
+      <c r="AGS25" s="0"/>
+      <c r="AGT25" s="0"/>
+      <c r="AGU25" s="0"/>
+      <c r="AGV25" s="0"/>
+      <c r="AGW25" s="0"/>
+      <c r="AGX25" s="0"/>
+      <c r="AGY25" s="0"/>
+      <c r="AGZ25" s="0"/>
+      <c r="AHA25" s="0"/>
+      <c r="AHB25" s="0"/>
+      <c r="AHC25" s="0"/>
+      <c r="AHD25" s="0"/>
+      <c r="AHE25" s="0"/>
+      <c r="AHF25" s="0"/>
+      <c r="AHG25" s="0"/>
+      <c r="AHH25" s="0"/>
+      <c r="AHI25" s="0"/>
+      <c r="AHJ25" s="0"/>
+      <c r="AHK25" s="0"/>
+      <c r="AHL25" s="0"/>
+      <c r="AHM25" s="0"/>
+      <c r="AHN25" s="0"/>
+      <c r="AHO25" s="0"/>
+      <c r="AHP25" s="0"/>
+      <c r="AHQ25" s="0"/>
+      <c r="AHR25" s="0"/>
+      <c r="AHS25" s="0"/>
+      <c r="AHT25" s="0"/>
+      <c r="AHU25" s="0"/>
+      <c r="AHV25" s="0"/>
+      <c r="AHW25" s="0"/>
+      <c r="AHX25" s="0"/>
+      <c r="AHY25" s="0"/>
+      <c r="AHZ25" s="0"/>
+      <c r="AIA25" s="0"/>
+      <c r="AIB25" s="0"/>
+      <c r="AIC25" s="0"/>
+      <c r="AID25" s="0"/>
+      <c r="AIE25" s="0"/>
+      <c r="AIF25" s="0"/>
+      <c r="AIG25" s="0"/>
+      <c r="AIH25" s="0"/>
+      <c r="AII25" s="0"/>
+      <c r="AIJ25" s="0"/>
+      <c r="AIK25" s="0"/>
+      <c r="AIL25" s="0"/>
+      <c r="AIM25" s="0"/>
+      <c r="AIN25" s="0"/>
+      <c r="AIO25" s="0"/>
+      <c r="AIP25" s="0"/>
+      <c r="AIQ25" s="0"/>
+      <c r="AIR25" s="0"/>
+      <c r="AIS25" s="0"/>
+      <c r="AIT25" s="0"/>
+      <c r="AIU25" s="0"/>
+      <c r="AIV25" s="0"/>
+      <c r="AIW25" s="0"/>
+      <c r="AIX25" s="0"/>
+      <c r="AIY25" s="0"/>
+      <c r="AIZ25" s="0"/>
+      <c r="AJA25" s="0"/>
+      <c r="AJB25" s="0"/>
+      <c r="AJC25" s="0"/>
+      <c r="AJD25" s="0"/>
+      <c r="AJE25" s="0"/>
+      <c r="AJF25" s="0"/>
+      <c r="AJG25" s="0"/>
+      <c r="AJH25" s="0"/>
+      <c r="AJI25" s="0"/>
+      <c r="AJJ25" s="0"/>
+      <c r="AJK25" s="0"/>
+      <c r="AJL25" s="0"/>
+      <c r="AJM25" s="0"/>
+      <c r="AJN25" s="0"/>
+      <c r="AJO25" s="0"/>
+      <c r="AJP25" s="0"/>
+      <c r="AJQ25" s="0"/>
+      <c r="AJR25" s="0"/>
+      <c r="AJS25" s="0"/>
+      <c r="AJT25" s="0"/>
+      <c r="AJU25" s="0"/>
+      <c r="AJV25" s="0"/>
+      <c r="AJW25" s="0"/>
+      <c r="AJX25" s="0"/>
+      <c r="AJY25" s="0"/>
+      <c r="AJZ25" s="0"/>
+      <c r="AKA25" s="0"/>
+      <c r="AKB25" s="0"/>
+      <c r="AKC25" s="0"/>
+      <c r="AKD25" s="0"/>
+      <c r="AKE25" s="0"/>
+      <c r="AKF25" s="0"/>
+      <c r="AKG25" s="0"/>
+      <c r="AKH25" s="0"/>
+      <c r="AKI25" s="0"/>
+      <c r="AKJ25" s="0"/>
+      <c r="AKK25" s="0"/>
+      <c r="AKL25" s="0"/>
+      <c r="AKM25" s="0"/>
+      <c r="AKN25" s="0"/>
+      <c r="AKO25" s="0"/>
+      <c r="AKP25" s="0"/>
+      <c r="AKQ25" s="0"/>
+      <c r="AKR25" s="0"/>
+      <c r="AKS25" s="0"/>
+      <c r="AKT25" s="0"/>
+      <c r="AKU25" s="0"/>
+      <c r="AKV25" s="0"/>
+      <c r="AKW25" s="0"/>
+      <c r="AKX25" s="0"/>
+      <c r="AKY25" s="0"/>
+      <c r="AKZ25" s="0"/>
+      <c r="ALA25" s="0"/>
+      <c r="ALB25" s="0"/>
+      <c r="ALC25" s="0"/>
+      <c r="ALD25" s="0"/>
+      <c r="ALE25" s="0"/>
+      <c r="ALF25" s="0"/>
+      <c r="ALG25" s="0"/>
+      <c r="ALH25" s="0"/>
+      <c r="ALI25" s="0"/>
+      <c r="ALJ25" s="0"/>
+      <c r="ALK25" s="0"/>
+      <c r="ALL25" s="0"/>
+      <c r="ALM25" s="0"/>
+      <c r="ALN25" s="0"/>
+      <c r="ALO25" s="0"/>
+      <c r="ALP25" s="0"/>
+      <c r="ALQ25" s="0"/>
+      <c r="ALR25" s="0"/>
+      <c r="ALS25" s="0"/>
+      <c r="ALT25" s="0"/>
+      <c r="ALU25" s="0"/>
+      <c r="ALV25" s="0"/>
+      <c r="ALW25" s="0"/>
+      <c r="ALX25" s="0"/>
+      <c r="ALY25" s="0"/>
+      <c r="ALZ25" s="0"/>
+      <c r="AMA25" s="0"/>
+      <c r="AMB25" s="0"/>
+      <c r="AMC25" s="0"/>
+      <c r="AMD25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+    <row r="26" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="0"/>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3" t="s">
+      <c r="F26" s="27"/>
+      <c r="G26" s="27" t="s">
         <v>41</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
-      <c r="K26" s="34"/>
+      <c r="K26" s="29"/>
+      <c r="AME26" s="29"/>
+      <c r="AMF26" s="29"/>
+      <c r="AMG26" s="0"/>
+      <c r="AMH26" s="0"/>
+      <c r="AMI26" s="0"/>
+      <c r="AMJ26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+      <c r="K27" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A2:B2"/>
@@ -24171,10 +23152,12 @@
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.379861111111111" right="0.379861111111111" top="0.645138888888889" bottom="0.645138888888889" header="0.379861111111111" footer="0.379861111111111"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>